<commit_message>
Changed crowd mic names
</commit_message>
<xml_diff>
--- a/Input List/Input List.xlsx
+++ b/Input List/Input List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TechnicalDocumentation\Input List\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dev\TechnicalDocumentation\Input List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAC95A96-D6E4-4DC7-8693-3B7C4A5828C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{796FD793-8F82-4DB3-BC39-BC409A6310F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
   </bookViews>
   <sheets>
     <sheet name="Input + Equipment" sheetId="1" r:id="rId1"/>
@@ -255,12 +255,6 @@
     <t>Vox</t>
   </si>
   <si>
-    <t>Crowd Mic Left</t>
-  </si>
-  <si>
-    <t>Crowd Mic Right</t>
-  </si>
-  <si>
     <t>Rodes</t>
   </si>
   <si>
@@ -442,6 +436,12 @@
   </si>
   <si>
     <t>Group Vox</t>
+  </si>
+  <si>
+    <t>Crowd Mic Ride</t>
+  </si>
+  <si>
+    <t>Crowd Mic Hi-Hat</t>
   </si>
 </sst>
 </file>
@@ -1001,6 +1001,90 @@
     <xf numFmtId="0" fontId="8" fillId="27" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1010,21 +1094,6 @@
     <xf numFmtId="0" fontId="15" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1040,164 +1109,95 @@
     <xf numFmtId="0" fontId="4" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1530,7 +1530,7 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1538,7 +1538,7 @@
     <col min="1" max="1" width="8.85546875" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" customWidth="1"/>
     <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
@@ -1549,10 +1549,10 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>58</v>
@@ -1577,10 +1577,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
-        <v>121</v>
-      </c>
-      <c r="B2" s="39" t="s">
+      <c r="A2" s="51" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="51" t="s">
         <v>69</v>
       </c>
       <c r="C2" s="13">
@@ -1598,12 +1598,12 @@
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
       <c r="I2" s="13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="40"/>
-      <c r="B3" s="40"/>
+      <c r="A3" s="52"/>
+      <c r="B3" s="52"/>
       <c r="C3" s="14">
         <v>2</v>
       </c>
@@ -1621,8 +1621,8 @@
       <c r="I3" s="14"/>
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
+      <c r="A4" s="52"/>
+      <c r="B4" s="52"/>
       <c r="C4" s="13">
         <v>3</v>
       </c>
@@ -1637,15 +1637,15 @@
       </c>
       <c r="G4" s="13"/>
       <c r="H4" s="13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="40"/>
-      <c r="B5" s="40"/>
+      <c r="A5" s="52"/>
+      <c r="B5" s="52"/>
       <c r="C5" s="14">
         <v>4</v>
       </c>
@@ -1660,15 +1660,15 @@
       </c>
       <c r="G5" s="14"/>
       <c r="H5" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="40"/>
-      <c r="B6" s="40"/>
+      <c r="A6" s="52"/>
+      <c r="B6" s="52"/>
       <c r="C6" s="13">
         <v>5</v>
       </c>
@@ -1683,15 +1683,15 @@
       </c>
       <c r="G6" s="13"/>
       <c r="H6" s="13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="40"/>
-      <c r="B7" s="40"/>
+      <c r="A7" s="52"/>
+      <c r="B7" s="52"/>
       <c r="C7" s="14">
         <v>6</v>
       </c>
@@ -1706,15 +1706,15 @@
       </c>
       <c r="G7" s="14"/>
       <c r="H7" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="40"/>
-      <c r="B8" s="40"/>
+      <c r="A8" s="52"/>
+      <c r="B8" s="52"/>
       <c r="C8" s="13">
         <v>7</v>
       </c>
@@ -1729,20 +1729,20 @@
       </c>
       <c r="G8" s="13"/>
       <c r="H8" s="13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="40"/>
-      <c r="B9" s="40"/>
+      <c r="A9" s="52"/>
+      <c r="B9" s="52"/>
       <c r="C9" s="14">
         <v>8</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>68</v>
@@ -1752,20 +1752,20 @@
       </c>
       <c r="G9" s="14"/>
       <c r="H9" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="40"/>
-      <c r="B10" s="40"/>
+      <c r="A10" s="52"/>
+      <c r="B10" s="52"/>
       <c r="C10" s="13">
         <v>9</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E10" s="13" t="s">
         <v>68</v>
@@ -1775,30 +1775,30 @@
       </c>
       <c r="G10" s="13"/>
       <c r="H10" s="13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="40"/>
-      <c r="B11" s="40"/>
+      <c r="A11" s="52"/>
+      <c r="B11" s="52"/>
       <c r="C11" s="14">
         <v>10</v>
       </c>
-      <c r="D11" s="58" t="s">
+      <c r="D11" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="E11" s="59"/>
-      <c r="F11" s="59"/>
-      <c r="G11" s="59"/>
-      <c r="H11" s="59"/>
-      <c r="I11" s="60"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="44"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="41"/>
-      <c r="B12" s="41"/>
+      <c r="A12" s="53"/>
+      <c r="B12" s="53"/>
       <c r="C12" s="13">
         <v>11</v>
       </c>
@@ -1809,18 +1809,18 @@
         <v>64</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="42" t="s">
-        <v>122</v>
-      </c>
-      <c r="B13" s="42" t="s">
-        <v>82</v>
+      <c r="A13" s="54" t="s">
+        <v>120</v>
+      </c>
+      <c r="B13" s="54" t="s">
+        <v>80</v>
       </c>
       <c r="C13" s="22">
         <v>12</v>
@@ -1829,26 +1829,26 @@
         <v>22</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G13" s="22"/>
       <c r="H13" s="22"/>
       <c r="I13" s="22"/>
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="43"/>
-      <c r="B14" s="43"/>
+      <c r="A14" s="55"/>
+      <c r="B14" s="55"/>
       <c r="C14" s="23">
         <v>13</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E14" s="23" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F14" s="23" t="s">
         <v>60</v>
@@ -1858,40 +1858,40 @@
       <c r="I14" s="23"/>
     </row>
     <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="44"/>
-      <c r="B15" s="67" t="s">
-        <v>86</v>
+      <c r="A15" s="67"/>
+      <c r="B15" s="56" t="s">
+        <v>84</v>
       </c>
       <c r="C15" s="19">
         <v>14</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G15" s="19"/>
       <c r="H15" s="19"/>
       <c r="I15" s="19"/>
     </row>
     <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="45"/>
-      <c r="B16" s="68"/>
+      <c r="A16" s="68"/>
+      <c r="B16" s="57"/>
       <c r="C16" s="20">
         <v>15</v>
       </c>
       <c r="D16" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="E16" s="20" t="s">
-        <v>79</v>
-      </c>
       <c r="F16" s="20" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G16" s="20"/>
       <c r="H16" s="20"/>
@@ -1900,110 +1900,110 @@
     <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="28"/>
       <c r="B17" s="29" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C17" s="18">
         <v>16</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>73</v>
+        <v>133</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F17" s="18" t="s">
         <v>60</v>
       </c>
       <c r="G17" s="18"/>
       <c r="H17" s="18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I17" s="18" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="35" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B18" s="34" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C18" s="33">
         <v>17</v>
       </c>
       <c r="D18" s="33" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E18" s="33"/>
       <c r="F18" s="33" t="s">
         <v>60</v>
       </c>
       <c r="G18" s="33" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H18" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="I18" s="33" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="61" t="s">
+        <v>121</v>
+      </c>
+      <c r="B19" s="61" t="s">
         <v>89</v>
-      </c>
-      <c r="I18" s="33" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="49" t="s">
-        <v>123</v>
-      </c>
-      <c r="B19" s="49" t="s">
-        <v>91</v>
       </c>
       <c r="C19" s="31">
         <v>18</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E19" s="31"/>
       <c r="F19" s="31" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G19" s="31" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H19" s="31"/>
       <c r="I19" s="31"/>
     </row>
     <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="50"/>
-      <c r="B20" s="50"/>
+      <c r="A20" s="62"/>
+      <c r="B20" s="62"/>
       <c r="C20" s="32">
         <v>19</v>
       </c>
-      <c r="D20" s="69" t="s">
+      <c r="D20" s="58" t="s">
         <v>70</v>
       </c>
-      <c r="E20" s="70"/>
-      <c r="F20" s="70"/>
-      <c r="G20" s="70"/>
-      <c r="H20" s="70"/>
-      <c r="I20" s="71"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="59"/>
+      <c r="G20" s="59"/>
+      <c r="H20" s="59"/>
+      <c r="I20" s="60"/>
     </row>
     <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="51"/>
-      <c r="B21" s="51"/>
+      <c r="A21" s="63"/>
+      <c r="B21" s="63"/>
       <c r="C21" s="31">
         <v>20</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E21" s="31" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F21" s="31" t="s">
         <v>60</v>
       </c>
       <c r="G21" s="31" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H21" s="31"/>
       <c r="I21" s="31"/>
@@ -2014,21 +2014,21 @@
       <c r="C22" s="25">
         <v>21</v>
       </c>
-      <c r="D22" s="61" t="s">
+      <c r="D22" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="E22" s="62"/>
-      <c r="F22" s="62"/>
-      <c r="G22" s="62"/>
-      <c r="H22" s="62"/>
-      <c r="I22" s="63"/>
+      <c r="E22" s="46"/>
+      <c r="F22" s="46"/>
+      <c r="G22" s="46"/>
+      <c r="H22" s="46"/>
+      <c r="I22" s="47"/>
     </row>
     <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="46" t="s">
-        <v>124</v>
-      </c>
-      <c r="B23" s="52" t="s">
-        <v>90</v>
+      <c r="A23" s="69" t="s">
+        <v>122</v>
+      </c>
+      <c r="B23" s="36" t="s">
+        <v>88</v>
       </c>
       <c r="C23" s="26">
         <v>22</v>
@@ -2037,68 +2037,68 @@
         <v>2</v>
       </c>
       <c r="E23" s="26" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F23" s="26" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G23" s="26" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H23" s="26"/>
       <c r="I23" s="26"/>
     </row>
     <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="47"/>
-      <c r="B24" s="53"/>
+      <c r="A24" s="70"/>
+      <c r="B24" s="37"/>
       <c r="C24" s="27">
         <v>23</v>
       </c>
       <c r="D24" s="27" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E24" s="27"/>
       <c r="F24" s="27" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G24" s="27" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H24" s="27"/>
       <c r="I24" s="27"/>
     </row>
     <row r="25" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="47"/>
-      <c r="B25" s="53"/>
+      <c r="A25" s="70"/>
+      <c r="B25" s="37"/>
       <c r="C25" s="26">
         <v>24</v>
       </c>
-      <c r="D25" s="64" t="s">
+      <c r="D25" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="E25" s="65"/>
-      <c r="F25" s="65"/>
-      <c r="G25" s="65"/>
-      <c r="H25" s="65"/>
-      <c r="I25" s="66"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="50"/>
     </row>
     <row r="26" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="48"/>
-      <c r="B26" s="54"/>
+      <c r="A26" s="71"/>
+      <c r="B26" s="38"/>
       <c r="C26" s="27">
         <v>25</v>
       </c>
       <c r="D26" s="27" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E26" s="27" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F26" s="27" t="s">
         <v>60</v>
       </c>
       <c r="G26" s="27" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H26" s="27"/>
       <c r="I26" s="27"/>
@@ -2109,21 +2109,21 @@
       <c r="C27" s="25">
         <v>26</v>
       </c>
-      <c r="D27" s="61" t="s">
+      <c r="D27" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="E27" s="62"/>
-      <c r="F27" s="62"/>
-      <c r="G27" s="62"/>
-      <c r="H27" s="62"/>
-      <c r="I27" s="63"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="46"/>
+      <c r="H27" s="46"/>
+      <c r="I27" s="47"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="B28" s="55" t="s">
-        <v>83</v>
+      <c r="A28" s="64" t="s">
+        <v>123</v>
+      </c>
+      <c r="B28" s="39" t="s">
+        <v>81</v>
       </c>
       <c r="C28" s="16">
         <v>27</v>
@@ -2133,121 +2133,127 @@
       </c>
       <c r="E28" s="16"/>
       <c r="F28" s="16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G28" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H28" s="16"/>
       <c r="I28" s="16"/>
     </row>
     <row r="29" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="37"/>
-      <c r="B29" s="56"/>
+      <c r="A29" s="65"/>
+      <c r="B29" s="40"/>
       <c r="C29" s="17">
         <v>28</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E29" s="17"/>
       <c r="F29" s="17" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G29" s="17" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H29" s="17"/>
       <c r="I29" s="17"/>
     </row>
     <row r="30" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="37"/>
-      <c r="B30" s="56"/>
+      <c r="A30" s="65"/>
+      <c r="B30" s="40"/>
       <c r="C30" s="16">
         <v>29</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E30" s="16"/>
       <c r="F30" s="16" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G30" s="16" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H30" s="16"/>
       <c r="I30" s="16"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="37"/>
-      <c r="B31" s="56"/>
+      <c r="A31" s="65"/>
+      <c r="B31" s="40"/>
       <c r="C31" s="17">
         <v>30</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E31" s="17"/>
       <c r="F31" s="17" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G31" s="17" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H31" s="17"/>
       <c r="I31" s="17"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="38"/>
-      <c r="B32" s="57"/>
+      <c r="A32" s="66"/>
+      <c r="B32" s="41"/>
       <c r="C32" s="16">
         <v>31</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F32" s="16" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G32" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H32" s="16"/>
       <c r="I32" s="16"/>
     </row>
-    <row r="33" spans="1:9" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="28"/>
       <c r="B33" s="30" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C33" s="18">
         <v>32</v>
       </c>
       <c r="D33" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="E33" s="18" t="s">
         <v>72</v>
-      </c>
-      <c r="E33" s="18" t="s">
-        <v>74</v>
       </c>
       <c r="F33" s="18" t="s">
         <v>60</v>
       </c>
       <c r="G33" s="18" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H33" s="18" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I33" s="18" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A28:A32"/>
+    <mergeCell ref="A2:A12"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A19:A21"/>
     <mergeCell ref="B23:B26"/>
     <mergeCell ref="B28:B32"/>
     <mergeCell ref="D11:I11"/>
@@ -2259,12 +2265,6 @@
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="D20:I20"/>
     <mergeCell ref="B19:B21"/>
-    <mergeCell ref="A28:A32"/>
-    <mergeCell ref="A2:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A19:A21"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2277,7 +2277,7 @@
   <dimension ref="A1:S34"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:H5"/>
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2291,40 +2291,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="75" t="s">
+      <c r="A1" s="89" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
+      <c r="F1" s="89"/>
+      <c r="G1" s="89"/>
+      <c r="H1" s="89"/>
       <c r="I1" s="3"/>
-      <c r="K1" s="93" t="s">
+      <c r="K1" s="86" t="s">
         <v>48</v>
       </c>
-      <c r="L1" s="93"/>
-      <c r="M1" s="93"/>
+      <c r="L1" s="86"/>
+      <c r="M1" s="86"/>
       <c r="N1" s="3"/>
-      <c r="P1" s="88" t="s">
+      <c r="P1" s="95" t="s">
         <v>42</v>
       </c>
-      <c r="Q1" s="88"/>
-      <c r="R1" s="88"/>
+      <c r="Q1" s="95"/>
+      <c r="R1" s="95"/>
     </row>
     <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
       <c r="I2" s="3"/>
       <c r="K2" s="5" t="s">
         <v>49</v>
@@ -2334,9 +2334,9 @@
         <v>50</v>
       </c>
       <c r="N2" s="3"/>
-      <c r="P2" s="88"/>
-      <c r="Q2" s="88"/>
-      <c r="R2" s="88"/>
+      <c r="P2" s="95"/>
+      <c r="Q2" s="95"/>
+      <c r="R2" s="95"/>
     </row>
     <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -2364,94 +2364,94 @@
         <v>8</v>
       </c>
       <c r="I3" s="3"/>
-      <c r="K3" s="87" t="s">
+      <c r="K3" s="72" t="s">
         <v>30</v>
       </c>
-      <c r="L3" s="87"/>
-      <c r="M3" s="87"/>
+      <c r="L3" s="72"/>
+      <c r="M3" s="72"/>
       <c r="N3" s="3"/>
-      <c r="P3" s="86" t="s">
+      <c r="P3" s="96" t="s">
         <v>35</v>
       </c>
-      <c r="Q3" s="90" t="s">
+      <c r="Q3" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="R3" s="86" t="s">
+      <c r="R3" s="96" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="78" t="s">
+      <c r="B4" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="78" t="s">
+      <c r="C4" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="78" t="s">
+      <c r="D4" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="79" t="s">
+      <c r="E4" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="79" t="s">
+      <c r="F4" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="79" t="s">
+      <c r="G4" s="78" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="78" t="s">
-        <v>128</v>
+      <c r="H4" s="80" t="s">
+        <v>126</v>
       </c>
       <c r="I4" s="3"/>
-      <c r="K4" s="84" t="s">
+      <c r="K4" s="97" t="s">
         <v>47</v>
       </c>
       <c r="L4" s="11">
         <v>1</v>
       </c>
-      <c r="M4" s="85" t="s">
+      <c r="M4" s="98" t="s">
         <v>51</v>
       </c>
       <c r="N4" s="3"/>
-      <c r="P4" s="86"/>
-      <c r="Q4" s="90"/>
-      <c r="R4" s="86"/>
+      <c r="P4" s="96"/>
+      <c r="Q4" s="76"/>
+      <c r="R4" s="96"/>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="78"/>
-      <c r="B5" s="78"/>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="80"/>
-      <c r="F5" s="80"/>
-      <c r="G5" s="80"/>
-      <c r="H5" s="78"/>
+      <c r="A5" s="80"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
+      <c r="H5" s="80"/>
       <c r="I5" s="3"/>
-      <c r="K5" s="84"/>
+      <c r="K5" s="97"/>
       <c r="L5" s="12">
         <v>3</v>
       </c>
-      <c r="M5" s="85"/>
+      <c r="M5" s="98"/>
       <c r="N5" s="3"/>
-      <c r="P5" s="86"/>
-      <c r="Q5" s="90"/>
-      <c r="R5" s="86"/>
+      <c r="P5" s="96"/>
+      <c r="Q5" s="76"/>
+      <c r="R5" s="96"/>
     </row>
     <row r="6" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I6" s="3"/>
-      <c r="K6" s="87" t="s">
-        <v>102</v>
-      </c>
-      <c r="L6" s="87"/>
-      <c r="M6" s="87"/>
+      <c r="K6" s="72" t="s">
+        <v>100</v>
+      </c>
+      <c r="L6" s="72"/>
+      <c r="M6" s="72"/>
       <c r="N6" s="3"/>
       <c r="P6" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="Q6" s="90"/>
+      <c r="Q6" s="76"/>
       <c r="R6" s="7" t="s">
         <v>27</v>
       </c>
@@ -2482,115 +2482,115 @@
         <v>16</v>
       </c>
       <c r="I7" s="3"/>
-      <c r="K7" s="84" t="s">
+      <c r="K7" s="97" t="s">
         <v>47</v>
       </c>
       <c r="L7" s="11">
         <v>2</v>
       </c>
-      <c r="M7" s="85" t="s">
+      <c r="M7" s="98" t="s">
         <v>51</v>
       </c>
       <c r="N7" s="3"/>
     </row>
     <row r="8" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="78" t="s">
-        <v>129</v>
-      </c>
-      <c r="B8" s="74"/>
-      <c r="C8" s="78" t="s">
+      <c r="A8" s="80" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" s="82"/>
+      <c r="C8" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="99" t="s">
+      <c r="D8" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="99" t="s">
+      <c r="E8" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="100" t="s">
-        <v>104</v>
-      </c>
-      <c r="G8" s="100" t="s">
-        <v>105</v>
-      </c>
-      <c r="H8" s="94" t="s">
+      <c r="F8" s="84" t="s">
+        <v>102</v>
+      </c>
+      <c r="G8" s="84" t="s">
+        <v>103</v>
+      </c>
+      <c r="H8" s="77" t="s">
         <v>23</v>
       </c>
       <c r="I8" s="3"/>
-      <c r="K8" s="84"/>
+      <c r="K8" s="97"/>
       <c r="L8" s="12">
         <v>2</v>
       </c>
-      <c r="M8" s="85"/>
+      <c r="M8" s="98"/>
       <c r="N8" s="3"/>
-      <c r="P8" s="86" t="s">
+      <c r="P8" s="96" t="s">
         <v>55</v>
       </c>
-      <c r="Q8" s="90" t="s">
+      <c r="Q8" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="R8" s="86" t="s">
+      <c r="R8" s="96" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="78"/>
-      <c r="B9" s="74"/>
-      <c r="C9" s="78"/>
-      <c r="D9" s="99"/>
-      <c r="E9" s="99"/>
-      <c r="F9" s="101"/>
-      <c r="G9" s="101"/>
-      <c r="H9" s="94"/>
+      <c r="A9" s="80"/>
+      <c r="B9" s="82"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="81"/>
+      <c r="E9" s="81"/>
+      <c r="F9" s="85"/>
+      <c r="G9" s="85"/>
+      <c r="H9" s="77"/>
       <c r="I9" s="3"/>
-      <c r="K9" s="87" t="s">
+      <c r="K9" s="72" t="s">
         <v>45</v>
       </c>
-      <c r="L9" s="87"/>
-      <c r="M9" s="87"/>
+      <c r="L9" s="72"/>
+      <c r="M9" s="72"/>
       <c r="N9" s="3"/>
-      <c r="P9" s="86"/>
-      <c r="Q9" s="90"/>
-      <c r="R9" s="86"/>
+      <c r="P9" s="96"/>
+      <c r="Q9" s="76"/>
+      <c r="R9" s="96"/>
     </row>
     <row r="10" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I10" s="3"/>
-      <c r="K10" s="84" t="s">
+      <c r="K10" s="97" t="s">
         <v>47</v>
       </c>
       <c r="L10" s="11">
         <v>3</v>
       </c>
-      <c r="M10" s="85" t="s">
+      <c r="M10" s="98" t="s">
         <v>51</v>
       </c>
       <c r="N10" s="3"/>
-      <c r="P10" s="86"/>
-      <c r="Q10" s="90"/>
-      <c r="R10" s="86"/>
+      <c r="P10" s="96"/>
+      <c r="Q10" s="76"/>
+      <c r="R10" s="96"/>
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="75" t="s">
+      <c r="A11" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="75"/>
-      <c r="C11" s="75"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="75"/>
-      <c r="G11" s="75"/>
-      <c r="H11" s="75"/>
+      <c r="B11" s="89"/>
+      <c r="C11" s="89"/>
+      <c r="D11" s="89"/>
+      <c r="E11" s="89"/>
+      <c r="F11" s="89"/>
+      <c r="G11" s="89"/>
+      <c r="H11" s="89"/>
       <c r="I11" s="3"/>
-      <c r="K11" s="84"/>
+      <c r="K11" s="97"/>
       <c r="L11" s="12">
         <v>1</v>
       </c>
-      <c r="M11" s="85"/>
+      <c r="M11" s="98"/>
       <c r="N11" s="3"/>
       <c r="P11" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="Q11" s="90"/>
+      <c r="Q11" s="76"/>
       <c r="R11" s="7" t="s">
         <v>29</v>
       </c>
@@ -2621,28 +2621,28 @@
         <v>8</v>
       </c>
       <c r="I12" s="3"/>
-      <c r="K12" s="87" t="s">
+      <c r="K12" s="72" t="s">
         <v>46</v>
       </c>
-      <c r="L12" s="87"/>
-      <c r="M12" s="87"/>
+      <c r="L12" s="72"/>
+      <c r="M12" s="72"/>
       <c r="N12" s="3"/>
     </row>
     <row r="13" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="79" t="s">
+      <c r="A13" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="78" t="s">
+      <c r="B13" s="80" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="99" t="s">
+      <c r="C13" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="74"/>
-      <c r="H13" s="77" t="s">
+      <c r="D13" s="82"/>
+      <c r="E13" s="82"/>
+      <c r="F13" s="82"/>
+      <c r="G13" s="82"/>
+      <c r="H13" s="83" t="s">
         <v>24</v>
       </c>
       <c r="I13" s="3"/>
@@ -2657,14 +2657,14 @@
       <c r="R13" s="2"/>
     </row>
     <row r="14" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="80"/>
-      <c r="B14" s="78"/>
-      <c r="C14" s="99"/>
-      <c r="D14" s="74"/>
-      <c r="E14" s="74"/>
-      <c r="F14" s="74"/>
-      <c r="G14" s="74"/>
-      <c r="H14" s="77"/>
+      <c r="A14" s="79"/>
+      <c r="B14" s="80"/>
+      <c r="C14" s="81"/>
+      <c r="D14" s="82"/>
+      <c r="E14" s="82"/>
+      <c r="F14" s="82"/>
+      <c r="G14" s="82"/>
+      <c r="H14" s="83"/>
       <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2677,80 +2677,80 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="3"/>
-      <c r="K15" s="88" t="s">
+      <c r="K15" s="95" t="s">
         <v>43</v>
       </c>
-      <c r="L15" s="88"/>
-      <c r="M15" s="88"/>
-      <c r="N15" s="88"/>
-      <c r="O15" s="88"/>
-      <c r="P15" s="88"/>
-      <c r="Q15" s="88"/>
+      <c r="L15" s="95"/>
+      <c r="M15" s="95"/>
+      <c r="N15" s="95"/>
+      <c r="O15" s="95"/>
+      <c r="P15" s="95"/>
+      <c r="Q15" s="95"/>
     </row>
     <row r="16" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I16" s="3"/>
-      <c r="K16" s="87" t="s">
+      <c r="K16" s="72" t="s">
         <v>55</v>
       </c>
-      <c r="L16" s="90" t="s">
+      <c r="L16" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="M16" s="87" t="s">
+      <c r="M16" s="72" t="s">
         <v>40</v>
       </c>
-      <c r="O16" s="87" t="s">
+      <c r="O16" s="72" t="s">
         <v>40</v>
       </c>
-      <c r="P16" s="90" t="s">
+      <c r="P16" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="Q16" s="87" t="s">
+      <c r="Q16" s="72" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="75" t="s">
+      <c r="A17" s="89" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="75"/>
-      <c r="C17" s="75"/>
-      <c r="D17" s="75"/>
-      <c r="E17" s="75"/>
-      <c r="F17" s="75"/>
-      <c r="G17" s="75"/>
-      <c r="H17" s="75"/>
+      <c r="B17" s="89"/>
+      <c r="C17" s="89"/>
+      <c r="D17" s="89"/>
+      <c r="E17" s="89"/>
+      <c r="F17" s="89"/>
+      <c r="G17" s="89"/>
+      <c r="H17" s="89"/>
       <c r="I17" s="3"/>
-      <c r="K17" s="89"/>
-      <c r="L17" s="90"/>
-      <c r="M17" s="87"/>
-      <c r="O17" s="87"/>
-      <c r="P17" s="90"/>
-      <c r="Q17" s="87"/>
+      <c r="K17" s="75"/>
+      <c r="L17" s="76"/>
+      <c r="M17" s="72"/>
+      <c r="O17" s="72"/>
+      <c r="P17" s="76"/>
+      <c r="Q17" s="72"/>
     </row>
     <row r="18" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="75" t="s">
+      <c r="A18" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="75"/>
-      <c r="C18" s="75"/>
-      <c r="D18" s="75"/>
-      <c r="E18" s="75"/>
-      <c r="F18" s="75"/>
-      <c r="G18" s="75"/>
-      <c r="H18" s="75"/>
+      <c r="B18" s="89"/>
+      <c r="C18" s="89"/>
+      <c r="D18" s="89"/>
+      <c r="E18" s="89"/>
+      <c r="F18" s="89"/>
+      <c r="G18" s="89"/>
+      <c r="H18" s="89"/>
       <c r="I18" s="3"/>
-      <c r="K18" s="91" t="s">
+      <c r="K18" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="L18" s="90"/>
-      <c r="M18" s="91" t="s">
+      <c r="L18" s="76"/>
+      <c r="M18" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="O18" s="91" t="s">
+      <c r="O18" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="P18" s="90"/>
-      <c r="Q18" s="91" t="s">
+      <c r="P18" s="76"/>
+      <c r="Q18" s="73" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2780,74 +2780,74 @@
         <v>8</v>
       </c>
       <c r="I19" s="3"/>
-      <c r="K19" s="92"/>
-      <c r="L19" s="90"/>
-      <c r="M19" s="92"/>
-      <c r="O19" s="92"/>
-      <c r="P19" s="90"/>
-      <c r="Q19" s="92"/>
+      <c r="K19" s="74"/>
+      <c r="L19" s="76"/>
+      <c r="M19" s="74"/>
+      <c r="O19" s="74"/>
+      <c r="P19" s="76"/>
+      <c r="Q19" s="74"/>
     </row>
     <row r="20" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="95" t="s">
-        <v>134</v>
-      </c>
-      <c r="B20" s="96" t="s">
-        <v>133</v>
-      </c>
-      <c r="C20" s="81"/>
-      <c r="D20" s="97" t="s">
-        <v>119</v>
-      </c>
-      <c r="E20" s="74"/>
-      <c r="F20" s="82" t="s">
+      <c r="A20" s="90" t="s">
+        <v>132</v>
+      </c>
+      <c r="B20" s="91" t="s">
+        <v>131</v>
+      </c>
+      <c r="C20" s="92"/>
+      <c r="D20" s="93" t="s">
+        <v>117</v>
+      </c>
+      <c r="E20" s="82"/>
+      <c r="F20" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="G20" s="82" t="s">
+      <c r="G20" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="H20" s="82"/>
+      <c r="H20" s="88"/>
       <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="95"/>
-      <c r="B21" s="96"/>
-      <c r="C21" s="81"/>
-      <c r="D21" s="98"/>
-      <c r="E21" s="74"/>
-      <c r="F21" s="82"/>
-      <c r="G21" s="82"/>
-      <c r="H21" s="82"/>
+      <c r="A21" s="90"/>
+      <c r="B21" s="91"/>
+      <c r="C21" s="92"/>
+      <c r="D21" s="94"/>
+      <c r="E21" s="82"/>
+      <c r="F21" s="88"/>
+      <c r="G21" s="88"/>
+      <c r="H21" s="88"/>
       <c r="I21" s="3"/>
-      <c r="K21" s="87" t="s">
+      <c r="K21" s="72" t="s">
         <v>35</v>
       </c>
-      <c r="L21" s="90" t="s">
+      <c r="L21" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="M21" s="87" t="s">
+      <c r="M21" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="O21" s="87" t="s">
+      <c r="O21" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="P21" s="90" t="s">
+      <c r="P21" s="76" t="s">
         <v>28</v>
       </c>
-      <c r="Q21" s="87" t="s">
+      <c r="Q21" s="72" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F22" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I22" s="3"/>
-      <c r="K22" s="87"/>
-      <c r="L22" s="90"/>
-      <c r="M22" s="87"/>
-      <c r="O22" s="87"/>
-      <c r="P22" s="90"/>
-      <c r="Q22" s="87"/>
+      <c r="K22" s="72"/>
+      <c r="L22" s="76"/>
+      <c r="M22" s="72"/>
+      <c r="O22" s="72"/>
+      <c r="P22" s="76"/>
+      <c r="Q22" s="72"/>
     </row>
     <row r="23" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
@@ -2875,68 +2875,68 @@
         <v>16</v>
       </c>
       <c r="I23" s="3"/>
-      <c r="K23" s="89"/>
-      <c r="L23" s="90"/>
-      <c r="M23" s="87"/>
-      <c r="O23" s="87"/>
-      <c r="P23" s="90"/>
-      <c r="Q23" s="87"/>
+      <c r="K23" s="75"/>
+      <c r="L23" s="76"/>
+      <c r="M23" s="72"/>
+      <c r="O23" s="72"/>
+      <c r="P23" s="76"/>
+      <c r="Q23" s="72"/>
     </row>
     <row r="24" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="82" t="s">
+      <c r="A24" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="74"/>
-      <c r="C24" s="83" t="s">
+      <c r="B24" s="82"/>
+      <c r="C24" s="87" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="83" t="s">
+      <c r="D24" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="E24" s="83" t="s">
+      <c r="E24" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="F24" s="83" t="s">
+      <c r="F24" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="G24" s="83" t="s">
+      <c r="G24" s="87" t="s">
         <v>3</v>
       </c>
-      <c r="H24" s="94" t="s">
+      <c r="H24" s="77" t="s">
         <v>10</v>
       </c>
       <c r="I24" s="3"/>
-      <c r="K24" s="91" t="s">
+      <c r="K24" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="L24" s="90"/>
-      <c r="M24" s="91" t="s">
+      <c r="L24" s="76"/>
+      <c r="M24" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="O24" s="91" t="s">
+      <c r="O24" s="73" t="s">
         <v>44</v>
       </c>
-      <c r="P24" s="90"/>
-      <c r="Q24" s="91" t="s">
+      <c r="P24" s="76"/>
+      <c r="Q24" s="73" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="82"/>
-      <c r="B25" s="74"/>
-      <c r="C25" s="83"/>
-      <c r="D25" s="83"/>
-      <c r="E25" s="83"/>
-      <c r="F25" s="83"/>
-      <c r="G25" s="83"/>
-      <c r="H25" s="94"/>
+      <c r="A25" s="88"/>
+      <c r="B25" s="82"/>
+      <c r="C25" s="87"/>
+      <c r="D25" s="87"/>
+      <c r="E25" s="87"/>
+      <c r="F25" s="87"/>
+      <c r="G25" s="87"/>
+      <c r="H25" s="77"/>
       <c r="I25" s="3"/>
-      <c r="K25" s="92"/>
-      <c r="L25" s="90"/>
-      <c r="M25" s="92"/>
-      <c r="O25" s="92"/>
-      <c r="P25" s="90"/>
-      <c r="Q25" s="92"/>
+      <c r="K25" s="74"/>
+      <c r="L25" s="76"/>
+      <c r="M25" s="74"/>
+      <c r="O25" s="74"/>
+      <c r="P25" s="76"/>
+      <c r="Q25" s="74"/>
     </row>
     <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I26" s="3"/>
@@ -2948,16 +2948,16 @@
       <c r="Q26" s="4"/>
     </row>
     <row r="27" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="75" t="s">
+      <c r="A27" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="75"/>
-      <c r="C27" s="75"/>
-      <c r="D27" s="75"/>
-      <c r="E27" s="75"/>
-      <c r="F27" s="75"/>
-      <c r="G27" s="75"/>
-      <c r="H27" s="75"/>
+      <c r="B27" s="89"/>
+      <c r="C27" s="89"/>
+      <c r="D27" s="89"/>
+      <c r="E27" s="89"/>
+      <c r="F27" s="89"/>
+      <c r="G27" s="89"/>
+      <c r="H27" s="89"/>
       <c r="I27" s="3"/>
       <c r="J27" s="10"/>
       <c r="K27" s="2"/>
@@ -2995,146 +2995,204 @@
         <v>8</v>
       </c>
       <c r="I28" s="3"/>
-      <c r="K28" s="76" t="s">
+      <c r="K28" s="99" t="s">
         <v>31</v>
       </c>
-      <c r="L28" s="76"/>
-      <c r="M28" s="76"/>
-      <c r="N28" s="76"/>
-      <c r="O28" s="76"/>
-      <c r="P28" s="76"/>
-      <c r="Q28" s="76"/>
-      <c r="R28" s="76"/>
+      <c r="L28" s="99"/>
+      <c r="M28" s="99"/>
+      <c r="N28" s="99"/>
+      <c r="O28" s="99"/>
+      <c r="P28" s="99"/>
+      <c r="Q28" s="99"/>
+      <c r="R28" s="99"/>
     </row>
     <row r="29" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="81" t="s">
+      <c r="A29" s="92" t="s">
         <v>57</v>
       </c>
-      <c r="B29" s="74"/>
-      <c r="C29" s="82" t="s">
+      <c r="B29" s="82"/>
+      <c r="C29" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="74"/>
-      <c r="E29" s="83" t="s">
+      <c r="D29" s="82"/>
+      <c r="E29" s="87" t="s">
         <v>26</v>
       </c>
-      <c r="F29" s="74"/>
-      <c r="G29" s="74"/>
-      <c r="H29" s="77" t="s">
+      <c r="F29" s="82"/>
+      <c r="G29" s="82"/>
+      <c r="H29" s="83" t="s">
         <v>9</v>
       </c>
       <c r="I29" s="3"/>
       <c r="K29" s="21">
         <v>1</v>
       </c>
-      <c r="L29" s="73" t="s">
+      <c r="L29" s="100" t="s">
         <v>32</v>
       </c>
-      <c r="M29" s="73"/>
-      <c r="N29" s="73"/>
-      <c r="O29" s="73"/>
-      <c r="P29" s="73"/>
-      <c r="Q29" s="73"/>
-      <c r="R29" s="73"/>
+      <c r="M29" s="100"/>
+      <c r="N29" s="100"/>
+      <c r="O29" s="100"/>
+      <c r="P29" s="100"/>
+      <c r="Q29" s="100"/>
+      <c r="R29" s="100"/>
     </row>
     <row r="30" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="81"/>
-      <c r="B30" s="74"/>
-      <c r="C30" s="82"/>
-      <c r="D30" s="74"/>
-      <c r="E30" s="83"/>
-      <c r="F30" s="74"/>
-      <c r="G30" s="74"/>
-      <c r="H30" s="77"/>
+      <c r="A30" s="92"/>
+      <c r="B30" s="82"/>
+      <c r="C30" s="88"/>
+      <c r="D30" s="82"/>
+      <c r="E30" s="87"/>
+      <c r="F30" s="82"/>
+      <c r="G30" s="82"/>
+      <c r="H30" s="83"/>
       <c r="I30" s="3"/>
       <c r="K30" s="8">
         <v>2</v>
       </c>
-      <c r="L30" s="72" t="s">
+      <c r="L30" s="101" t="s">
         <v>33</v>
       </c>
-      <c r="M30" s="72"/>
-      <c r="N30" s="72"/>
-      <c r="O30" s="72"/>
-      <c r="P30" s="72"/>
-      <c r="Q30" s="72"/>
-      <c r="R30" s="72"/>
+      <c r="M30" s="101"/>
+      <c r="N30" s="101"/>
+      <c r="O30" s="101"/>
+      <c r="P30" s="101"/>
+      <c r="Q30" s="101"/>
+      <c r="R30" s="101"/>
     </row>
     <row r="31" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I31" s="3"/>
       <c r="K31" s="21">
         <v>3</v>
       </c>
-      <c r="L31" s="73" t="s">
+      <c r="L31" s="100" t="s">
         <v>52</v>
       </c>
-      <c r="M31" s="73"/>
-      <c r="N31" s="73"/>
-      <c r="O31" s="73"/>
-      <c r="P31" s="73"/>
-      <c r="Q31" s="73"/>
-      <c r="R31" s="73"/>
+      <c r="M31" s="100"/>
+      <c r="N31" s="100"/>
+      <c r="O31" s="100"/>
+      <c r="P31" s="100"/>
+      <c r="Q31" s="100"/>
+      <c r="R31" s="100"/>
     </row>
     <row r="32" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I32" s="3"/>
       <c r="K32" s="8">
         <v>4</v>
       </c>
-      <c r="L32" s="72" t="s">
+      <c r="L32" s="101" t="s">
         <v>53</v>
       </c>
-      <c r="M32" s="72"/>
-      <c r="N32" s="72"/>
-      <c r="O32" s="72"/>
-      <c r="P32" s="72"/>
-      <c r="Q32" s="72"/>
-      <c r="R32" s="72"/>
+      <c r="M32" s="101"/>
+      <c r="N32" s="101"/>
+      <c r="O32" s="101"/>
+      <c r="P32" s="101"/>
+      <c r="Q32" s="101"/>
+      <c r="R32" s="101"/>
     </row>
     <row r="33" spans="9:18" x14ac:dyDescent="0.25">
       <c r="I33" s="3"/>
       <c r="K33" s="21">
         <v>5</v>
       </c>
-      <c r="L33" s="73" t="s">
+      <c r="L33" s="100" t="s">
         <v>54</v>
       </c>
-      <c r="M33" s="73"/>
-      <c r="N33" s="73"/>
-      <c r="O33" s="73"/>
-      <c r="P33" s="73"/>
-      <c r="Q33" s="73"/>
-      <c r="R33" s="73"/>
+      <c r="M33" s="100"/>
+      <c r="N33" s="100"/>
+      <c r="O33" s="100"/>
+      <c r="P33" s="100"/>
+      <c r="Q33" s="100"/>
+      <c r="R33" s="100"/>
     </row>
     <row r="34" spans="9:18" x14ac:dyDescent="0.25">
       <c r="I34" s="3"/>
       <c r="K34" s="8">
         <v>5</v>
       </c>
-      <c r="L34" s="72" t="s">
+      <c r="L34" s="101" t="s">
         <v>56</v>
       </c>
-      <c r="M34" s="72"/>
-      <c r="N34" s="72"/>
-      <c r="O34" s="72"/>
-      <c r="P34" s="72"/>
-      <c r="Q34" s="72"/>
-      <c r="R34" s="72"/>
+      <c r="M34" s="101"/>
+      <c r="N34" s="101"/>
+      <c r="O34" s="101"/>
+      <c r="P34" s="101"/>
+      <c r="Q34" s="101"/>
+      <c r="R34" s="101"/>
     </row>
   </sheetData>
   <mergeCells count="100">
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="O24:O25"/>
-    <mergeCell ref="Q24:Q25"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="Q18:Q19"/>
-    <mergeCell ref="K21:K23"/>
-    <mergeCell ref="L21:L25"/>
-    <mergeCell ref="O21:O23"/>
-    <mergeCell ref="P21:P25"/>
-    <mergeCell ref="Q21:Q23"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="M24:M25"/>
-    <mergeCell ref="M21:M23"/>
+    <mergeCell ref="L32:R32"/>
+    <mergeCell ref="L33:R33"/>
+    <mergeCell ref="L34:R34"/>
+    <mergeCell ref="L29:R29"/>
+    <mergeCell ref="L30:R30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="K28:R28"/>
+    <mergeCell ref="L31:R31"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="R3:R5"/>
+    <mergeCell ref="P3:P5"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="P1:R2"/>
+    <mergeCell ref="K15:Q15"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="L16:L19"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="O16:O17"/>
+    <mergeCell ref="P16:P19"/>
+    <mergeCell ref="Q16:Q17"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="P8:P10"/>
+    <mergeCell ref="Q8:Q11"/>
+    <mergeCell ref="Q3:Q6"/>
+    <mergeCell ref="R8:R10"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="K3:M3"/>
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="B13:B14"/>
@@ -3151,77 +3209,19 @@
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="F8:F9"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="A18:H18"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="P1:R2"/>
-    <mergeCell ref="K15:Q15"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="L16:L19"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="O16:O17"/>
-    <mergeCell ref="P16:P19"/>
-    <mergeCell ref="Q16:Q17"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="P8:P10"/>
-    <mergeCell ref="Q8:Q11"/>
-    <mergeCell ref="Q3:Q6"/>
-    <mergeCell ref="R8:R10"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="M10:M11"/>
-    <mergeCell ref="R3:R5"/>
-    <mergeCell ref="P3:P5"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="A11:H11"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="K28:R28"/>
-    <mergeCell ref="L31:R31"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="L32:R32"/>
-    <mergeCell ref="L33:R33"/>
-    <mergeCell ref="L34:R34"/>
-    <mergeCell ref="L29:R29"/>
-    <mergeCell ref="L30:R30"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="O24:O25"/>
+    <mergeCell ref="Q24:Q25"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="Q18:Q19"/>
+    <mergeCell ref="K21:K23"/>
+    <mergeCell ref="L21:L25"/>
+    <mergeCell ref="O21:O23"/>
+    <mergeCell ref="P21:P25"/>
+    <mergeCell ref="Q21:Q23"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="M21:M23"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added John Aux. Moved John Vox.
</commit_message>
<xml_diff>
--- a/Input List/Input List.xlsx
+++ b/Input List/Input List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dev\TechnicalDocumentation\Input List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{796FD793-8F82-4DB3-BC39-BC409A6310F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{222C3438-8B68-4E27-9DED-9691015FC917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
   </bookViews>
   <sheets>
     <sheet name="Input + Equipment" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="134">
   <si>
     <t>Input</t>
   </si>
@@ -261,12 +261,6 @@
     <t>John Vox</t>
   </si>
   <si>
-    <t>Bluetooth Left</t>
-  </si>
-  <si>
-    <t>Bluetooth Right</t>
-  </si>
-  <si>
     <t>Shure Beta 58</t>
   </si>
   <si>
@@ -345,12 +339,6 @@
     <t>48V Phantom power provided by FOH</t>
   </si>
   <si>
-    <t>BT Left</t>
-  </si>
-  <si>
-    <t>BT Right</t>
-  </si>
-  <si>
     <t>Front.1</t>
   </si>
   <si>
@@ -442,13 +430,22 @@
   </si>
   <si>
     <t>Crowd Mic Hi-Hat</t>
+  </si>
+  <si>
+    <t>John Aux</t>
+  </si>
+  <si>
+    <t>DI Box</t>
+  </si>
+  <si>
+    <t>Blue Tooth</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -605,6 +602,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13.5"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -934,7 +939,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -970,7 +975,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1001,6 +1005,48 @@
     <xf numFmtId="0" fontId="8" fillId="27" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1046,27 +1092,6 @@
     <xf numFmtId="0" fontId="12" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="26" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1076,128 +1101,113 @@
     <xf numFmtId="0" fontId="0" fillId="26" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1231,9 +1241,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1271,7 +1281,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1377,7 +1387,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1519,7 +1529,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1529,8 +1539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18A11D25-D77D-4358-9E34-E04B11CA4C7B}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="P25" sqref="P25"/>
+    <sheetView topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1549,10 +1559,10 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>58</v>
@@ -1577,10 +1587,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="51" t="s">
-        <v>119</v>
-      </c>
-      <c r="B2" s="51" t="s">
+      <c r="A2" s="38" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" s="38" t="s">
         <v>69</v>
       </c>
       <c r="C2" s="13">
@@ -1598,12 +1608,12 @@
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
       <c r="I2" s="13" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="52"/>
-      <c r="B3" s="52"/>
+      <c r="A3" s="39"/>
+      <c r="B3" s="39"/>
       <c r="C3" s="14">
         <v>2</v>
       </c>
@@ -1621,8 +1631,8 @@
       <c r="I3" s="14"/>
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="52"/>
-      <c r="B4" s="52"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="39"/>
       <c r="C4" s="13">
         <v>3</v>
       </c>
@@ -1637,15 +1647,15 @@
       </c>
       <c r="G4" s="13"/>
       <c r="H4" s="13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="52"/>
-      <c r="B5" s="52"/>
+      <c r="A5" s="39"/>
+      <c r="B5" s="39"/>
       <c r="C5" s="14">
         <v>4</v>
       </c>
@@ -1660,15 +1670,15 @@
       </c>
       <c r="G5" s="14"/>
       <c r="H5" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="52"/>
-      <c r="B6" s="52"/>
+      <c r="A6" s="39"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="13">
         <v>5</v>
       </c>
@@ -1683,15 +1693,15 @@
       </c>
       <c r="G6" s="13"/>
       <c r="H6" s="13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="52"/>
-      <c r="B7" s="52"/>
+      <c r="A7" s="39"/>
+      <c r="B7" s="39"/>
       <c r="C7" s="14">
         <v>6</v>
       </c>
@@ -1706,15 +1716,15 @@
       </c>
       <c r="G7" s="14"/>
       <c r="H7" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="52"/>
-      <c r="B8" s="52"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="39"/>
       <c r="C8" s="13">
         <v>7</v>
       </c>
@@ -1729,20 +1739,20 @@
       </c>
       <c r="G8" s="13"/>
       <c r="H8" s="13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="52"/>
-      <c r="B9" s="52"/>
+      <c r="A9" s="39"/>
+      <c r="B9" s="39"/>
       <c r="C9" s="14">
         <v>8</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E9" s="14" t="s">
         <v>68</v>
@@ -1752,20 +1762,20 @@
       </c>
       <c r="G9" s="14"/>
       <c r="H9" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="52"/>
-      <c r="B10" s="52"/>
+      <c r="A10" s="39"/>
+      <c r="B10" s="39"/>
       <c r="C10" s="13">
         <v>9</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E10" s="13" t="s">
         <v>68</v>
@@ -1775,30 +1785,30 @@
       </c>
       <c r="G10" s="13"/>
       <c r="H10" s="13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="52"/>
-      <c r="B11" s="52"/>
+      <c r="A11" s="39"/>
+      <c r="B11" s="39"/>
       <c r="C11" s="14">
         <v>10</v>
       </c>
-      <c r="D11" s="42" t="s">
+      <c r="D11" s="55" t="s">
         <v>70</v>
       </c>
-      <c r="E11" s="43"/>
-      <c r="F11" s="43"/>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43"/>
-      <c r="I11" s="44"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="56"/>
+      <c r="H11" s="56"/>
+      <c r="I11" s="57"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="53"/>
-      <c r="B12" s="53"/>
+      <c r="A12" s="40"/>
+      <c r="B12" s="40"/>
       <c r="C12" s="13">
         <v>11</v>
       </c>
@@ -1809,104 +1819,104 @@
         <v>64</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="54" t="s">
-        <v>120</v>
-      </c>
-      <c r="B13" s="54" t="s">
-        <v>80</v>
-      </c>
-      <c r="C13" s="22">
+      <c r="A13" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="B13" s="41" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="21">
         <v>12</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="F13" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
+      <c r="E13" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="55"/>
-      <c r="B14" s="55"/>
-      <c r="C14" s="23">
+      <c r="A14" s="99"/>
+      <c r="B14" s="99"/>
+      <c r="C14" s="22">
         <v>13</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="D14" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+    </row>
+    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="99"/>
+      <c r="B15" s="42"/>
+      <c r="C15" s="21">
+        <v>14</v>
+      </c>
+      <c r="D15" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="E14" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="F14" s="23" t="s">
+      <c r="E15" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="F15" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
-    </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="67"/>
-      <c r="B15" s="56" t="s">
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+    </row>
+    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="97"/>
+      <c r="B16" s="98" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="19">
+        <v>15</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="F16" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+    </row>
+    <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="27"/>
+      <c r="B17" s="28" t="s">
         <v>84</v>
-      </c>
-      <c r="C15" s="19">
-        <v>14</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="F15" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-    </row>
-    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="68"/>
-      <c r="B16" s="57"/>
-      <c r="C16" s="20">
-        <v>15</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="F16" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-    </row>
-    <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="28"/>
-      <c r="B17" s="29" t="s">
-        <v>86</v>
       </c>
       <c r="C17" s="18">
         <v>16</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E17" s="18" t="s">
         <v>72</v>
@@ -1916,214 +1926,218 @@
       </c>
       <c r="G17" s="18"/>
       <c r="H17" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="I17" s="18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" s="33" t="s">
+        <v>124</v>
+      </c>
+      <c r="C18" s="32">
+        <v>17</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="G18" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="H18" s="32" t="s">
+        <v>85</v>
+      </c>
+      <c r="I18" s="32" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="100" t="s">
+        <v>117</v>
+      </c>
+      <c r="B19" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="I17" s="18" t="s">
+      <c r="C19" s="30">
+        <v>18</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>127</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="F19" s="30" t="s">
+        <v>77</v>
+      </c>
+      <c r="G19" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
+    </row>
+    <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="101"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="31">
+        <v>19</v>
+      </c>
+      <c r="D20" s="64" t="s">
+        <v>70</v>
+      </c>
+      <c r="E20" s="65"/>
+      <c r="F20" s="65"/>
+      <c r="G20" s="65"/>
+      <c r="H20" s="65"/>
+      <c r="I20" s="66"/>
+    </row>
+    <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="102"/>
+      <c r="B21" s="48"/>
+      <c r="C21" s="30">
+        <v>20</v>
+      </c>
+      <c r="D21" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="E21" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="F21" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="G21" s="30" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="35" t="s">
-        <v>83</v>
-      </c>
-      <c r="B18" s="34" t="s">
-        <v>128</v>
-      </c>
-      <c r="C18" s="33">
-        <v>17</v>
-      </c>
-      <c r="D18" s="33" t="s">
-        <v>129</v>
-      </c>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33" t="s">
+      <c r="H21" s="30"/>
+      <c r="I21" s="30"/>
+    </row>
+    <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="27"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="24">
+        <v>21</v>
+      </c>
+      <c r="D22" s="58" t="s">
+        <v>70</v>
+      </c>
+      <c r="E22" s="59"/>
+      <c r="F22" s="59"/>
+      <c r="G22" s="59"/>
+      <c r="H22" s="59"/>
+      <c r="I22" s="60"/>
+    </row>
+    <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="43" t="s">
+        <v>118</v>
+      </c>
+      <c r="B23" s="49" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" s="25">
+        <v>22</v>
+      </c>
+      <c r="D23" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="F23" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="G23" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="H23" s="25"/>
+      <c r="I23" s="25"/>
+    </row>
+    <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="44"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="26">
+        <v>23</v>
+      </c>
+      <c r="D24" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="E24" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="F24" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="G24" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26"/>
+    </row>
+    <row r="25" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="44"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="25">
+        <v>24</v>
+      </c>
+      <c r="D25" s="61" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" s="62"/>
+      <c r="F25" s="62"/>
+      <c r="G25" s="62"/>
+      <c r="H25" s="62"/>
+      <c r="I25" s="63"/>
+    </row>
+    <row r="26" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="45"/>
+      <c r="B26" s="51"/>
+      <c r="C26" s="26">
+        <v>25</v>
+      </c>
+      <c r="D26" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="E26" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="F26" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="G18" s="33" t="s">
+      <c r="G26" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="H18" s="33" t="s">
-        <v>87</v>
-      </c>
-      <c r="I18" s="33" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="61" t="s">
-        <v>121</v>
-      </c>
-      <c r="B19" s="61" t="s">
-        <v>89</v>
-      </c>
-      <c r="C19" s="31">
-        <v>18</v>
-      </c>
-      <c r="D19" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31" t="s">
+      <c r="H26" s="26"/>
+      <c r="I26" s="26"/>
+    </row>
+    <row r="27" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="27"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="24">
+        <v>26</v>
+      </c>
+      <c r="D27" s="58" t="s">
+        <v>70</v>
+      </c>
+      <c r="E27" s="59"/>
+      <c r="F27" s="59"/>
+      <c r="G27" s="59"/>
+      <c r="H27" s="59"/>
+      <c r="I27" s="60"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="35" t="s">
+        <v>119</v>
+      </c>
+      <c r="B28" s="52" t="s">
         <v>79</v>
-      </c>
-      <c r="G19" s="31" t="s">
-        <v>130</v>
-      </c>
-      <c r="H19" s="31"/>
-      <c r="I19" s="31"/>
-    </row>
-    <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="62"/>
-      <c r="B20" s="62"/>
-      <c r="C20" s="32">
-        <v>19</v>
-      </c>
-      <c r="D20" s="58" t="s">
-        <v>70</v>
-      </c>
-      <c r="E20" s="59"/>
-      <c r="F20" s="59"/>
-      <c r="G20" s="59"/>
-      <c r="H20" s="59"/>
-      <c r="I20" s="60"/>
-    </row>
-    <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="63"/>
-      <c r="B21" s="63"/>
-      <c r="C21" s="31">
-        <v>20</v>
-      </c>
-      <c r="D21" s="31" t="s">
-        <v>115</v>
-      </c>
-      <c r="E21" s="31" t="s">
-        <v>116</v>
-      </c>
-      <c r="F21" s="31" t="s">
-        <v>60</v>
-      </c>
-      <c r="G21" s="31" t="s">
-        <v>105</v>
-      </c>
-      <c r="H21" s="31"/>
-      <c r="I21" s="31"/>
-    </row>
-    <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="28"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="25">
-        <v>21</v>
-      </c>
-      <c r="D22" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="E22" s="46"/>
-      <c r="F22" s="46"/>
-      <c r="G22" s="46"/>
-      <c r="H22" s="46"/>
-      <c r="I22" s="47"/>
-    </row>
-    <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="69" t="s">
-        <v>122</v>
-      </c>
-      <c r="B23" s="36" t="s">
-        <v>88</v>
-      </c>
-      <c r="C23" s="26">
-        <v>22</v>
-      </c>
-      <c r="D23" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="E23" s="26" t="s">
-        <v>94</v>
-      </c>
-      <c r="F23" s="26" t="s">
-        <v>99</v>
-      </c>
-      <c r="G23" s="26" t="s">
-        <v>106</v>
-      </c>
-      <c r="H23" s="26"/>
-      <c r="I23" s="26"/>
-    </row>
-    <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="70"/>
-      <c r="B24" s="37"/>
-      <c r="C24" s="27">
-        <v>23</v>
-      </c>
-      <c r="D24" s="27" t="s">
-        <v>93</v>
-      </c>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="G24" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="H24" s="27"/>
-      <c r="I24" s="27"/>
-    </row>
-    <row r="25" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="70"/>
-      <c r="B25" s="37"/>
-      <c r="C25" s="26">
-        <v>24</v>
-      </c>
-      <c r="D25" s="48" t="s">
-        <v>70</v>
-      </c>
-      <c r="E25" s="49"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="49"/>
-      <c r="H25" s="49"/>
-      <c r="I25" s="50"/>
-    </row>
-    <row r="26" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="71"/>
-      <c r="B26" s="38"/>
-      <c r="C26" s="27">
-        <v>25</v>
-      </c>
-      <c r="D26" s="27" t="s">
-        <v>90</v>
-      </c>
-      <c r="E26" s="27" t="s">
-        <v>91</v>
-      </c>
-      <c r="F26" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="G26" s="27" t="s">
-        <v>108</v>
-      </c>
-      <c r="H26" s="27"/>
-      <c r="I26" s="27"/>
-    </row>
-    <row r="27" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="28"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="25">
-        <v>26</v>
-      </c>
-      <c r="D27" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="E27" s="46"/>
-      <c r="F27" s="46"/>
-      <c r="G27" s="46"/>
-      <c r="H27" s="46"/>
-      <c r="I27" s="47"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="64" t="s">
-        <v>123</v>
-      </c>
-      <c r="B28" s="39" t="s">
-        <v>81</v>
       </c>
       <c r="C28" s="16">
         <v>27</v>
@@ -2133,102 +2147,104 @@
       </c>
       <c r="E28" s="16"/>
       <c r="F28" s="16" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G28" s="16" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H28" s="16"/>
       <c r="I28" s="16"/>
     </row>
     <row r="29" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="65"/>
-      <c r="B29" s="40"/>
+      <c r="A29" s="36"/>
+      <c r="B29" s="53"/>
       <c r="C29" s="17">
         <v>28</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E29" s="17"/>
       <c r="F29" s="17" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G29" s="17" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="H29" s="17"/>
       <c r="I29" s="17"/>
     </row>
     <row r="30" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="65"/>
-      <c r="B30" s="40"/>
+      <c r="A30" s="36"/>
+      <c r="B30" s="53"/>
       <c r="C30" s="16">
         <v>29</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E30" s="16"/>
       <c r="F30" s="16" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G30" s="16" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="H30" s="16"/>
       <c r="I30" s="16"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="65"/>
-      <c r="B31" s="40"/>
+      <c r="A31" s="36"/>
+      <c r="B31" s="53"/>
       <c r="C31" s="17">
         <v>30</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="E31" s="17"/>
+        <v>95</v>
+      </c>
+      <c r="E31" s="17" t="s">
+        <v>132</v>
+      </c>
       <c r="F31" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G31" s="17" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H31" s="17"/>
       <c r="I31" s="17"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="66"/>
-      <c r="B32" s="41"/>
+      <c r="A32" s="37"/>
+      <c r="B32" s="54"/>
       <c r="C32" s="16">
         <v>31</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F32" s="16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G32" s="16" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H32" s="16"/>
       <c r="I32" s="16"/>
     </row>
     <row r="33" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="28"/>
-      <c r="B33" s="30" t="s">
-        <v>86</v>
+      <c r="A33" s="27"/>
+      <c r="B33" s="29" t="s">
+        <v>84</v>
       </c>
       <c r="C33" s="18">
         <v>32</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E33" s="18" t="s">
         <v>72</v>
@@ -2237,23 +2253,17 @@
         <v>60</v>
       </c>
       <c r="G33" s="18" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H33" s="18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I33" s="18" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="A28:A32"/>
-    <mergeCell ref="A2:A12"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A19:A21"/>
+  <mergeCells count="15">
     <mergeCell ref="B23:B26"/>
     <mergeCell ref="B28:B32"/>
     <mergeCell ref="D11:I11"/>
@@ -2261,10 +2271,14 @@
     <mergeCell ref="D25:I25"/>
     <mergeCell ref="D27:I27"/>
     <mergeCell ref="B2:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B15:B16"/>
     <mergeCell ref="D20:I20"/>
     <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="A28:A32"/>
+    <mergeCell ref="A2:A12"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="A13:A15"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2276,8 +2290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{036672A4-8952-44C6-9E0D-0D4906E8D835}">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2291,40 +2305,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
       <c r="I1" s="3"/>
-      <c r="K1" s="86" t="s">
+      <c r="K1" s="88" t="s">
         <v>48</v>
       </c>
-      <c r="L1" s="86"/>
-      <c r="M1" s="86"/>
+      <c r="L1" s="88"/>
+      <c r="M1" s="88"/>
       <c r="N1" s="3"/>
-      <c r="P1" s="95" t="s">
+      <c r="P1" s="83" t="s">
         <v>42</v>
       </c>
-      <c r="Q1" s="95"/>
-      <c r="R1" s="95"/>
+      <c r="Q1" s="83"/>
+      <c r="R1" s="83"/>
     </row>
     <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="89"/>
-      <c r="C2" s="89"/>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
       <c r="I2" s="3"/>
       <c r="K2" s="5" t="s">
         <v>49</v>
@@ -2334,9 +2348,9 @@
         <v>50</v>
       </c>
       <c r="N2" s="3"/>
-      <c r="P2" s="95"/>
-      <c r="Q2" s="95"/>
-      <c r="R2" s="95"/>
+      <c r="P2" s="83"/>
+      <c r="Q2" s="83"/>
+      <c r="R2" s="83"/>
     </row>
     <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -2364,94 +2378,94 @@
         <v>8</v>
       </c>
       <c r="I3" s="3"/>
-      <c r="K3" s="72" t="s">
+      <c r="K3" s="82" t="s">
         <v>30</v>
       </c>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
+      <c r="L3" s="82"/>
+      <c r="M3" s="82"/>
       <c r="N3" s="3"/>
-      <c r="P3" s="96" t="s">
+      <c r="P3" s="81" t="s">
         <v>35</v>
       </c>
-      <c r="Q3" s="76" t="s">
+      <c r="Q3" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="R3" s="96" t="s">
+      <c r="R3" s="81" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="80" t="s">
+      <c r="A4" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="80" t="s">
+      <c r="B4" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="80" t="s">
+      <c r="C4" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="80" t="s">
+      <c r="D4" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="78" t="s">
+      <c r="E4" s="74" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="78" t="s">
+      <c r="F4" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="78" t="s">
+      <c r="G4" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="80" t="s">
-        <v>126</v>
+      <c r="H4" s="73" t="s">
+        <v>122</v>
       </c>
       <c r="I4" s="3"/>
-      <c r="K4" s="97" t="s">
+      <c r="K4" s="79" t="s">
         <v>47</v>
       </c>
       <c r="L4" s="11">
         <v>1</v>
       </c>
-      <c r="M4" s="98" t="s">
+      <c r="M4" s="80" t="s">
         <v>51</v>
       </c>
       <c r="N4" s="3"/>
-      <c r="P4" s="96"/>
-      <c r="Q4" s="76"/>
-      <c r="R4" s="96"/>
+      <c r="P4" s="81"/>
+      <c r="Q4" s="85"/>
+      <c r="R4" s="81"/>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="80"/>
-      <c r="B5" s="80"/>
-      <c r="C5" s="80"/>
-      <c r="D5" s="80"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="79"/>
-      <c r="G5" s="79"/>
-      <c r="H5" s="80"/>
+      <c r="A5" s="73"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="73"/>
       <c r="I5" s="3"/>
-      <c r="K5" s="97"/>
+      <c r="K5" s="79"/>
       <c r="L5" s="12">
         <v>3</v>
       </c>
-      <c r="M5" s="98"/>
+      <c r="M5" s="80"/>
       <c r="N5" s="3"/>
-      <c r="P5" s="96"/>
-      <c r="Q5" s="76"/>
-      <c r="R5" s="96"/>
+      <c r="P5" s="81"/>
+      <c r="Q5" s="85"/>
+      <c r="R5" s="81"/>
     </row>
     <row r="6" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I6" s="3"/>
-      <c r="K6" s="72" t="s">
-        <v>100</v>
-      </c>
-      <c r="L6" s="72"/>
-      <c r="M6" s="72"/>
+      <c r="K6" s="82" t="s">
+        <v>98</v>
+      </c>
+      <c r="L6" s="82"/>
+      <c r="M6" s="82"/>
       <c r="N6" s="3"/>
       <c r="P6" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="Q6" s="76"/>
+      <c r="Q6" s="85"/>
       <c r="R6" s="7" t="s">
         <v>27</v>
       </c>
@@ -2482,115 +2496,115 @@
         <v>16</v>
       </c>
       <c r="I7" s="3"/>
-      <c r="K7" s="97" t="s">
+      <c r="K7" s="79" t="s">
         <v>47</v>
       </c>
       <c r="L7" s="11">
         <v>2</v>
       </c>
-      <c r="M7" s="98" t="s">
+      <c r="M7" s="80" t="s">
         <v>51</v>
       </c>
       <c r="N7" s="3"/>
     </row>
     <row r="8" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="80" t="s">
-        <v>127</v>
-      </c>
-      <c r="B8" s="82"/>
-      <c r="C8" s="80" t="s">
+      <c r="A8" s="73" t="s">
+        <v>123</v>
+      </c>
+      <c r="B8" s="69"/>
+      <c r="C8" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="81" t="s">
+      <c r="D8" s="94" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="81" t="s">
+      <c r="E8" s="94" t="s">
+        <v>131</v>
+      </c>
+      <c r="F8" s="94" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="84" t="s">
-        <v>102</v>
-      </c>
-      <c r="G8" s="84" t="s">
-        <v>103</v>
-      </c>
-      <c r="H8" s="77" t="s">
+      <c r="G8" s="95" t="s">
+        <v>133</v>
+      </c>
+      <c r="H8" s="89" t="s">
         <v>23</v>
       </c>
       <c r="I8" s="3"/>
-      <c r="K8" s="97"/>
+      <c r="K8" s="79"/>
       <c r="L8" s="12">
         <v>2</v>
       </c>
-      <c r="M8" s="98"/>
+      <c r="M8" s="80"/>
       <c r="N8" s="3"/>
-      <c r="P8" s="96" t="s">
+      <c r="P8" s="81" t="s">
         <v>55</v>
       </c>
-      <c r="Q8" s="76" t="s">
+      <c r="Q8" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="R8" s="96" t="s">
+      <c r="R8" s="81" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="80"/>
-      <c r="B9" s="82"/>
-      <c r="C9" s="80"/>
-      <c r="D9" s="81"/>
-      <c r="E9" s="81"/>
-      <c r="F9" s="85"/>
-      <c r="G9" s="85"/>
-      <c r="H9" s="77"/>
+      <c r="A9" s="73"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="94"/>
+      <c r="E9" s="94"/>
+      <c r="F9" s="94"/>
+      <c r="G9" s="96"/>
+      <c r="H9" s="89"/>
       <c r="I9" s="3"/>
-      <c r="K9" s="72" t="s">
+      <c r="K9" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="L9" s="72"/>
-      <c r="M9" s="72"/>
+      <c r="L9" s="82"/>
+      <c r="M9" s="82"/>
       <c r="N9" s="3"/>
-      <c r="P9" s="96"/>
-      <c r="Q9" s="76"/>
-      <c r="R9" s="96"/>
+      <c r="P9" s="81"/>
+      <c r="Q9" s="85"/>
+      <c r="R9" s="81"/>
     </row>
     <row r="10" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I10" s="3"/>
-      <c r="K10" s="97" t="s">
+      <c r="K10" s="79" t="s">
         <v>47</v>
       </c>
       <c r="L10" s="11">
         <v>3</v>
       </c>
-      <c r="M10" s="98" t="s">
+      <c r="M10" s="80" t="s">
         <v>51</v>
       </c>
       <c r="N10" s="3"/>
-      <c r="P10" s="96"/>
-      <c r="Q10" s="76"/>
-      <c r="R10" s="96"/>
+      <c r="P10" s="81"/>
+      <c r="Q10" s="85"/>
+      <c r="R10" s="81"/>
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="89" t="s">
+      <c r="A11" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="89"/>
-      <c r="C11" s="89"/>
-      <c r="D11" s="89"/>
-      <c r="E11" s="89"/>
-      <c r="F11" s="89"/>
-      <c r="G11" s="89"/>
-      <c r="H11" s="89"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="70"/>
+      <c r="H11" s="70"/>
       <c r="I11" s="3"/>
-      <c r="K11" s="97"/>
+      <c r="K11" s="79"/>
       <c r="L11" s="12">
         <v>1</v>
       </c>
-      <c r="M11" s="98"/>
+      <c r="M11" s="80"/>
       <c r="N11" s="3"/>
       <c r="P11" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="Q11" s="76"/>
+      <c r="Q11" s="85"/>
       <c r="R11" s="7" t="s">
         <v>29</v>
       </c>
@@ -2621,28 +2635,28 @@
         <v>8</v>
       </c>
       <c r="I12" s="3"/>
-      <c r="K12" s="72" t="s">
+      <c r="K12" s="82" t="s">
         <v>46</v>
       </c>
-      <c r="L12" s="72"/>
-      <c r="M12" s="72"/>
+      <c r="L12" s="82"/>
+      <c r="M12" s="82"/>
       <c r="N12" s="3"/>
     </row>
     <row r="13" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="78" t="s">
+      <c r="A13" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="80" t="s">
+      <c r="B13" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="81" t="s">
+      <c r="C13" s="94" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="82"/>
-      <c r="E13" s="82"/>
-      <c r="F13" s="82"/>
-      <c r="G13" s="82"/>
-      <c r="H13" s="83" t="s">
+      <c r="D13" s="69"/>
+      <c r="E13" s="69"/>
+      <c r="F13" s="69"/>
+      <c r="G13" s="69"/>
+      <c r="H13" s="72" t="s">
         <v>24</v>
       </c>
       <c r="I13" s="3"/>
@@ -2657,14 +2671,14 @@
       <c r="R13" s="2"/>
     </row>
     <row r="14" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="79"/>
-      <c r="B14" s="80"/>
-      <c r="C14" s="81"/>
-      <c r="D14" s="82"/>
-      <c r="E14" s="82"/>
-      <c r="F14" s="82"/>
-      <c r="G14" s="82"/>
-      <c r="H14" s="83"/>
+      <c r="A14" s="75"/>
+      <c r="B14" s="73"/>
+      <c r="C14" s="94"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="69"/>
+      <c r="G14" s="69"/>
+      <c r="H14" s="72"/>
       <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2677,80 +2691,80 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="3"/>
-      <c r="K15" s="95" t="s">
+      <c r="K15" s="83" t="s">
         <v>43</v>
       </c>
-      <c r="L15" s="95"/>
-      <c r="M15" s="95"/>
-      <c r="N15" s="95"/>
-      <c r="O15" s="95"/>
-      <c r="P15" s="95"/>
-      <c r="Q15" s="95"/>
+      <c r="L15" s="83"/>
+      <c r="M15" s="83"/>
+      <c r="N15" s="83"/>
+      <c r="O15" s="83"/>
+      <c r="P15" s="83"/>
+      <c r="Q15" s="83"/>
     </row>
     <row r="16" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I16" s="3"/>
-      <c r="K16" s="72" t="s">
+      <c r="K16" s="82" t="s">
         <v>55</v>
       </c>
-      <c r="L16" s="76" t="s">
+      <c r="L16" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="M16" s="72" t="s">
+      <c r="M16" s="82" t="s">
         <v>40</v>
       </c>
-      <c r="O16" s="72" t="s">
+      <c r="O16" s="82" t="s">
         <v>40</v>
       </c>
-      <c r="P16" s="76" t="s">
+      <c r="P16" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="Q16" s="72" t="s">
+      <c r="Q16" s="82" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="89" t="s">
+      <c r="A17" s="70" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="89"/>
-      <c r="C17" s="89"/>
-      <c r="D17" s="89"/>
-      <c r="E17" s="89"/>
-      <c r="F17" s="89"/>
-      <c r="G17" s="89"/>
-      <c r="H17" s="89"/>
+      <c r="B17" s="70"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="70"/>
+      <c r="E17" s="70"/>
+      <c r="F17" s="70"/>
+      <c r="G17" s="70"/>
+      <c r="H17" s="70"/>
       <c r="I17" s="3"/>
-      <c r="K17" s="75"/>
-      <c r="L17" s="76"/>
-      <c r="M17" s="72"/>
-      <c r="O17" s="72"/>
-      <c r="P17" s="76"/>
-      <c r="Q17" s="72"/>
+      <c r="K17" s="84"/>
+      <c r="L17" s="85"/>
+      <c r="M17" s="82"/>
+      <c r="O17" s="82"/>
+      <c r="P17" s="85"/>
+      <c r="Q17" s="82"/>
     </row>
     <row r="18" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="89" t="s">
+      <c r="A18" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="89"/>
-      <c r="C18" s="89"/>
-      <c r="D18" s="89"/>
-      <c r="E18" s="89"/>
-      <c r="F18" s="89"/>
-      <c r="G18" s="89"/>
-      <c r="H18" s="89"/>
+      <c r="B18" s="70"/>
+      <c r="C18" s="70"/>
+      <c r="D18" s="70"/>
+      <c r="E18" s="70"/>
+      <c r="F18" s="70"/>
+      <c r="G18" s="70"/>
+      <c r="H18" s="70"/>
       <c r="I18" s="3"/>
-      <c r="K18" s="73" t="s">
+      <c r="K18" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="L18" s="76"/>
-      <c r="M18" s="73" t="s">
+      <c r="L18" s="85"/>
+      <c r="M18" s="86" t="s">
         <v>39</v>
       </c>
-      <c r="O18" s="73" t="s">
+      <c r="O18" s="86" t="s">
         <v>44</v>
       </c>
-      <c r="P18" s="76"/>
-      <c r="Q18" s="73" t="s">
+      <c r="P18" s="85"/>
+      <c r="Q18" s="86" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2780,74 +2794,74 @@
         <v>8</v>
       </c>
       <c r="I19" s="3"/>
-      <c r="K19" s="74"/>
-      <c r="L19" s="76"/>
-      <c r="M19" s="74"/>
-      <c r="O19" s="74"/>
-      <c r="P19" s="76"/>
-      <c r="Q19" s="74"/>
+      <c r="K19" s="87"/>
+      <c r="L19" s="85"/>
+      <c r="M19" s="87"/>
+      <c r="O19" s="87"/>
+      <c r="P19" s="85"/>
+      <c r="Q19" s="87"/>
     </row>
     <row r="20" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="90" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B20" s="91" t="s">
-        <v>131</v>
-      </c>
-      <c r="C20" s="92"/>
-      <c r="D20" s="93" t="s">
-        <v>117</v>
-      </c>
-      <c r="E20" s="82"/>
-      <c r="F20" s="88" t="s">
+        <v>127</v>
+      </c>
+      <c r="C20" s="76"/>
+      <c r="D20" s="92" t="s">
+        <v>113</v>
+      </c>
+      <c r="E20" s="69"/>
+      <c r="F20" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="G20" s="88" t="s">
+      <c r="G20" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="H20" s="88"/>
+      <c r="H20" s="77"/>
       <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="90"/>
       <c r="B21" s="91"/>
-      <c r="C21" s="92"/>
-      <c r="D21" s="94"/>
-      <c r="E21" s="82"/>
-      <c r="F21" s="88"/>
-      <c r="G21" s="88"/>
-      <c r="H21" s="88"/>
+      <c r="C21" s="76"/>
+      <c r="D21" s="93"/>
+      <c r="E21" s="69"/>
+      <c r="F21" s="77"/>
+      <c r="G21" s="77"/>
+      <c r="H21" s="77"/>
       <c r="I21" s="3"/>
-      <c r="K21" s="72" t="s">
+      <c r="K21" s="82" t="s">
         <v>35</v>
       </c>
-      <c r="L21" s="76" t="s">
+      <c r="L21" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="M21" s="72" t="s">
+      <c r="M21" s="82" t="s">
         <v>37</v>
       </c>
-      <c r="O21" s="72" t="s">
+      <c r="O21" s="82" t="s">
         <v>37</v>
       </c>
-      <c r="P21" s="76" t="s">
+      <c r="P21" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="Q21" s="72" t="s">
+      <c r="Q21" s="82" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="22" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F22" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I22" s="3"/>
-      <c r="K22" s="72"/>
-      <c r="L22" s="76"/>
-      <c r="M22" s="72"/>
-      <c r="O22" s="72"/>
-      <c r="P22" s="76"/>
-      <c r="Q22" s="72"/>
+      <c r="K22" s="82"/>
+      <c r="L22" s="85"/>
+      <c r="M22" s="82"/>
+      <c r="O22" s="82"/>
+      <c r="P22" s="85"/>
+      <c r="Q22" s="82"/>
     </row>
     <row r="23" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
@@ -2875,68 +2889,68 @@
         <v>16</v>
       </c>
       <c r="I23" s="3"/>
-      <c r="K23" s="75"/>
-      <c r="L23" s="76"/>
-      <c r="M23" s="72"/>
-      <c r="O23" s="72"/>
-      <c r="P23" s="76"/>
-      <c r="Q23" s="72"/>
+      <c r="K23" s="84"/>
+      <c r="L23" s="85"/>
+      <c r="M23" s="82"/>
+      <c r="O23" s="82"/>
+      <c r="P23" s="85"/>
+      <c r="Q23" s="82"/>
     </row>
     <row r="24" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="88" t="s">
+      <c r="A24" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="82"/>
-      <c r="C24" s="87" t="s">
+      <c r="B24" s="69"/>
+      <c r="C24" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="87" t="s">
+      <c r="D24" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="E24" s="87" t="s">
+      <c r="E24" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="F24" s="87" t="s">
+      <c r="F24" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="G24" s="87" t="s">
+      <c r="G24" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="H24" s="77" t="s">
+      <c r="H24" s="89" t="s">
         <v>10</v>
       </c>
       <c r="I24" s="3"/>
-      <c r="K24" s="73" t="s">
+      <c r="K24" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="L24" s="76"/>
-      <c r="M24" s="73" t="s">
+      <c r="L24" s="85"/>
+      <c r="M24" s="86" t="s">
         <v>39</v>
       </c>
-      <c r="O24" s="73" t="s">
+      <c r="O24" s="86" t="s">
         <v>44</v>
       </c>
-      <c r="P24" s="76"/>
-      <c r="Q24" s="73" t="s">
+      <c r="P24" s="85"/>
+      <c r="Q24" s="86" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="88"/>
-      <c r="B25" s="82"/>
-      <c r="C25" s="87"/>
-      <c r="D25" s="87"/>
-      <c r="E25" s="87"/>
-      <c r="F25" s="87"/>
-      <c r="G25" s="87"/>
-      <c r="H25" s="77"/>
+      <c r="A25" s="77"/>
+      <c r="B25" s="69"/>
+      <c r="C25" s="78"/>
+      <c r="D25" s="78"/>
+      <c r="E25" s="78"/>
+      <c r="F25" s="78"/>
+      <c r="G25" s="78"/>
+      <c r="H25" s="89"/>
       <c r="I25" s="3"/>
-      <c r="K25" s="74"/>
-      <c r="L25" s="76"/>
-      <c r="M25" s="74"/>
-      <c r="O25" s="74"/>
-      <c r="P25" s="76"/>
-      <c r="Q25" s="74"/>
+      <c r="K25" s="87"/>
+      <c r="L25" s="85"/>
+      <c r="M25" s="87"/>
+      <c r="O25" s="87"/>
+      <c r="P25" s="85"/>
+      <c r="Q25" s="87"/>
     </row>
     <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I26" s="3"/>
@@ -2948,16 +2962,16 @@
       <c r="Q26" s="4"/>
     </row>
     <row r="27" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="89" t="s">
+      <c r="A27" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="89"/>
-      <c r="C27" s="89"/>
-      <c r="D27" s="89"/>
-      <c r="E27" s="89"/>
-      <c r="F27" s="89"/>
-      <c r="G27" s="89"/>
-      <c r="H27" s="89"/>
+      <c r="B27" s="70"/>
+      <c r="C27" s="70"/>
+      <c r="D27" s="70"/>
+      <c r="E27" s="70"/>
+      <c r="F27" s="70"/>
+      <c r="G27" s="70"/>
+      <c r="H27" s="70"/>
       <c r="I27" s="3"/>
       <c r="J27" s="10"/>
       <c r="K27" s="2"/>
@@ -2995,138 +3009,212 @@
         <v>8</v>
       </c>
       <c r="I28" s="3"/>
-      <c r="K28" s="99" t="s">
+      <c r="K28" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="L28" s="99"/>
-      <c r="M28" s="99"/>
-      <c r="N28" s="99"/>
-      <c r="O28" s="99"/>
-      <c r="P28" s="99"/>
-      <c r="Q28" s="99"/>
-      <c r="R28" s="99"/>
+      <c r="L28" s="71"/>
+      <c r="M28" s="71"/>
+      <c r="N28" s="71"/>
+      <c r="O28" s="71"/>
+      <c r="P28" s="71"/>
+      <c r="Q28" s="71"/>
+      <c r="R28" s="71"/>
     </row>
     <row r="29" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="92" t="s">
+      <c r="A29" s="76" t="s">
         <v>57</v>
       </c>
-      <c r="B29" s="82"/>
-      <c r="C29" s="88" t="s">
+      <c r="B29" s="69"/>
+      <c r="C29" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="82"/>
-      <c r="E29" s="87" t="s">
+      <c r="D29" s="69"/>
+      <c r="E29" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="F29" s="82"/>
-      <c r="G29" s="82"/>
-      <c r="H29" s="83" t="s">
+      <c r="F29" s="69"/>
+      <c r="G29" s="69"/>
+      <c r="H29" s="72" t="s">
         <v>9</v>
       </c>
       <c r="I29" s="3"/>
-      <c r="K29" s="21">
+      <c r="K29" s="20">
         <v>1</v>
       </c>
-      <c r="L29" s="100" t="s">
+      <c r="L29" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="M29" s="100"/>
-      <c r="N29" s="100"/>
-      <c r="O29" s="100"/>
-      <c r="P29" s="100"/>
-      <c r="Q29" s="100"/>
-      <c r="R29" s="100"/>
+      <c r="M29" s="68"/>
+      <c r="N29" s="68"/>
+      <c r="O29" s="68"/>
+      <c r="P29" s="68"/>
+      <c r="Q29" s="68"/>
+      <c r="R29" s="68"/>
     </row>
     <row r="30" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="92"/>
-      <c r="B30" s="82"/>
-      <c r="C30" s="88"/>
-      <c r="D30" s="82"/>
-      <c r="E30" s="87"/>
-      <c r="F30" s="82"/>
-      <c r="G30" s="82"/>
-      <c r="H30" s="83"/>
+      <c r="A30" s="76"/>
+      <c r="B30" s="69"/>
+      <c r="C30" s="77"/>
+      <c r="D30" s="69"/>
+      <c r="E30" s="78"/>
+      <c r="F30" s="69"/>
+      <c r="G30" s="69"/>
+      <c r="H30" s="72"/>
       <c r="I30" s="3"/>
       <c r="K30" s="8">
         <v>2</v>
       </c>
-      <c r="L30" s="101" t="s">
+      <c r="L30" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="M30" s="101"/>
-      <c r="N30" s="101"/>
-      <c r="O30" s="101"/>
-      <c r="P30" s="101"/>
-      <c r="Q30" s="101"/>
-      <c r="R30" s="101"/>
+      <c r="M30" s="67"/>
+      <c r="N30" s="67"/>
+      <c r="O30" s="67"/>
+      <c r="P30" s="67"/>
+      <c r="Q30" s="67"/>
+      <c r="R30" s="67"/>
     </row>
     <row r="31" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I31" s="3"/>
-      <c r="K31" s="21">
+      <c r="K31" s="20">
         <v>3</v>
       </c>
-      <c r="L31" s="100" t="s">
+      <c r="L31" s="68" t="s">
         <v>52</v>
       </c>
-      <c r="M31" s="100"/>
-      <c r="N31" s="100"/>
-      <c r="O31" s="100"/>
-      <c r="P31" s="100"/>
-      <c r="Q31" s="100"/>
-      <c r="R31" s="100"/>
+      <c r="M31" s="68"/>
+      <c r="N31" s="68"/>
+      <c r="O31" s="68"/>
+      <c r="P31" s="68"/>
+      <c r="Q31" s="68"/>
+      <c r="R31" s="68"/>
     </row>
     <row r="32" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I32" s="3"/>
       <c r="K32" s="8">
         <v>4</v>
       </c>
-      <c r="L32" s="101" t="s">
+      <c r="L32" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="M32" s="101"/>
-      <c r="N32" s="101"/>
-      <c r="O32" s="101"/>
-      <c r="P32" s="101"/>
-      <c r="Q32" s="101"/>
-      <c r="R32" s="101"/>
+      <c r="M32" s="67"/>
+      <c r="N32" s="67"/>
+      <c r="O32" s="67"/>
+      <c r="P32" s="67"/>
+      <c r="Q32" s="67"/>
+      <c r="R32" s="67"/>
     </row>
     <row r="33" spans="9:18" x14ac:dyDescent="0.25">
       <c r="I33" s="3"/>
-      <c r="K33" s="21">
+      <c r="K33" s="20">
         <v>5</v>
       </c>
-      <c r="L33" s="100" t="s">
+      <c r="L33" s="68" t="s">
         <v>54</v>
       </c>
-      <c r="M33" s="100"/>
-      <c r="N33" s="100"/>
-      <c r="O33" s="100"/>
-      <c r="P33" s="100"/>
-      <c r="Q33" s="100"/>
-      <c r="R33" s="100"/>
+      <c r="M33" s="68"/>
+      <c r="N33" s="68"/>
+      <c r="O33" s="68"/>
+      <c r="P33" s="68"/>
+      <c r="Q33" s="68"/>
+      <c r="R33" s="68"/>
     </row>
     <row r="34" spans="9:18" x14ac:dyDescent="0.25">
       <c r="I34" s="3"/>
       <c r="K34" s="8">
         <v>5</v>
       </c>
-      <c r="L34" s="101" t="s">
+      <c r="L34" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="M34" s="101"/>
-      <c r="N34" s="101"/>
-      <c r="O34" s="101"/>
-      <c r="P34" s="101"/>
-      <c r="Q34" s="101"/>
-      <c r="R34" s="101"/>
+      <c r="M34" s="67"/>
+      <c r="N34" s="67"/>
+      <c r="O34" s="67"/>
+      <c r="P34" s="67"/>
+      <c r="Q34" s="67"/>
+      <c r="R34" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="100">
-    <mergeCell ref="L32:R32"/>
-    <mergeCell ref="L33:R33"/>
-    <mergeCell ref="L34:R34"/>
-    <mergeCell ref="L29:R29"/>
-    <mergeCell ref="L30:R30"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="O24:O25"/>
+    <mergeCell ref="Q24:Q25"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="Q18:Q19"/>
+    <mergeCell ref="K21:K23"/>
+    <mergeCell ref="L21:L25"/>
+    <mergeCell ref="O21:O23"/>
+    <mergeCell ref="P21:P25"/>
+    <mergeCell ref="Q21:Q23"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="M21:M23"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="P1:R2"/>
+    <mergeCell ref="K15:Q15"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="L16:L19"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="O16:O17"/>
+    <mergeCell ref="P16:P19"/>
+    <mergeCell ref="Q16:Q17"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="P8:P10"/>
+    <mergeCell ref="Q8:Q11"/>
+    <mergeCell ref="Q3:Q6"/>
+    <mergeCell ref="R8:R10"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="R3:R5"/>
+    <mergeCell ref="P3:P5"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
     <mergeCell ref="F29:F30"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:H2"/>
@@ -3143,85 +3231,11 @@
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="H4:H5"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="A11:H11"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="M10:M11"/>
-    <mergeCell ref="R3:R5"/>
-    <mergeCell ref="P3:P5"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="P1:R2"/>
-    <mergeCell ref="K15:Q15"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="L16:L19"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="O16:O17"/>
-    <mergeCell ref="P16:P19"/>
-    <mergeCell ref="Q16:Q17"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="P8:P10"/>
-    <mergeCell ref="Q8:Q11"/>
-    <mergeCell ref="Q3:Q6"/>
-    <mergeCell ref="R8:R10"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="A18:H18"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="O24:O25"/>
-    <mergeCell ref="Q24:Q25"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="Q18:Q19"/>
-    <mergeCell ref="K21:K23"/>
-    <mergeCell ref="L21:L25"/>
-    <mergeCell ref="O21:O23"/>
-    <mergeCell ref="P21:P25"/>
-    <mergeCell ref="Q21:Q23"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="M24:M25"/>
-    <mergeCell ref="M21:M23"/>
+    <mergeCell ref="L32:R32"/>
+    <mergeCell ref="L33:R33"/>
+    <mergeCell ref="L34:R34"/>
+    <mergeCell ref="L29:R29"/>
+    <mergeCell ref="L30:R30"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated stage diagram for new box
</commit_message>
<xml_diff>
--- a/Input List/Input List.xlsx
+++ b/Input List/Input List.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TechnicalDocumentation\Input List\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dev\TechnicalDocumentation\Input List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE19E2A-0E68-432A-8C35-36417ADEE3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAFBCBD1-C029-4C0B-A19C-75FEECA8B508}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="1" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
   </bookViews>
   <sheets>
     <sheet name="Input + Equipment" sheetId="1" r:id="rId1"/>
     <sheet name="Snake + PA" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="125">
   <si>
     <t>Input</t>
   </si>
@@ -199,15 +198,6 @@
     <t>Black cables are for utility (the PA and crowd mics)</t>
   </si>
   <si>
-    <t>Crowd mic cables are black with a right-angle connector</t>
-  </si>
-  <si>
-    <t>Front Snake</t>
-  </si>
-  <si>
-    <t>Use the Analog Snake to connect musicians to Front Box</t>
-  </si>
-  <si>
     <t>Channel</t>
   </si>
   <si>
@@ -247,15 +237,6 @@
     <t>Unused</t>
   </si>
   <si>
-    <t>Vox</t>
-  </si>
-  <si>
-    <t>Rodes</t>
-  </si>
-  <si>
-    <t>John Vox</t>
-  </si>
-  <si>
     <t>Shure Beta 58</t>
   </si>
   <si>
@@ -283,12 +264,6 @@
     <t>Bluetooth</t>
   </si>
   <si>
-    <t>Kenzi Vox</t>
-  </si>
-  <si>
-    <t>Crowd</t>
-  </si>
-  <si>
     <t>YES</t>
   </si>
   <si>
@@ -298,9 +273,6 @@
     <t>Guitar Right</t>
   </si>
   <si>
-    <t>Paul Vox</t>
-  </si>
-  <si>
     <t>Shure 55SH</t>
   </si>
   <si>
@@ -328,39 +300,6 @@
     <t>Amp Hang</t>
   </si>
   <si>
-    <t>Drum &amp; Front Boxes</t>
-  </si>
-  <si>
-    <t>48V Phantom power provided by FOH</t>
-  </si>
-  <si>
-    <t>Front.4</t>
-  </si>
-  <si>
-    <t>Front.6</t>
-  </si>
-  <si>
-    <t>Front.7</t>
-  </si>
-  <si>
-    <t>Front.9</t>
-  </si>
-  <si>
-    <t>Front.11</t>
-  </si>
-  <si>
-    <t>Front.12</t>
-  </si>
-  <si>
-    <t>Front.13</t>
-  </si>
-  <si>
-    <t>Front.14</t>
-  </si>
-  <si>
-    <t>Front.15</t>
-  </si>
-  <si>
     <t>Internally suspended inside bass drum</t>
   </si>
   <si>
@@ -403,13 +342,7 @@
     <t>Overhd Ride</t>
   </si>
   <si>
-    <t>Front.2</t>
-  </si>
-  <si>
     <t>Jessica Acoustic</t>
-  </si>
-  <si>
-    <t>Crowd Mic Hi-Hat</t>
   </si>
   <si>
     <t>John Aux</t>
@@ -435,6 +368,51 @@
   </si>
   <si>
     <t>Jess IEM</t>
+  </si>
+  <si>
+    <t>Use the Analog Snake to connect musicians to Mixer</t>
+  </si>
+  <si>
+    <t>IEM Box</t>
+  </si>
+  <si>
+    <t>Drum &amp; Bass Snake</t>
+  </si>
+  <si>
+    <t>Guitar &amp; Keyboards Snake</t>
+  </si>
+  <si>
+    <t>Guitar Snake</t>
+  </si>
+  <si>
+    <t>48V Phantom power provided by IEM Box</t>
+  </si>
+  <si>
+    <t>FrontSnake.2</t>
+  </si>
+  <si>
+    <t>FrontSnake.4</t>
+  </si>
+  <si>
+    <t>FrontSnake.6</t>
+  </si>
+  <si>
+    <t>FrontSnake.9</t>
+  </si>
+  <si>
+    <t>FrontSnake.11</t>
+  </si>
+  <si>
+    <t>FrontSnake.12</t>
+  </si>
+  <si>
+    <t>FrontSnake.13</t>
+  </si>
+  <si>
+    <t>FrontSnake.14</t>
+  </si>
+  <si>
+    <t>FrontSnake.15</t>
   </si>
 </sst>
 </file>
@@ -923,7 +901,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -974,19 +952,52 @@
     <xf numFmtId="0" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="25" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -1033,15 +1044,6 @@
     <xf numFmtId="0" fontId="12" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="25" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1060,56 +1062,83 @@
     <xf numFmtId="0" fontId="19" fillId="24" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1117,68 +1146,23 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1212,9 +1196,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1252,7 +1236,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1358,7 +1342,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1500,7 +1484,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1510,8 +1494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18A11D25-D77D-4358-9E34-E04B11CA4C7B}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView topLeftCell="A13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1530,39 +1514,39 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="15" t="s">
         <v>57</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="H1" s="15" t="s">
-        <v>60</v>
       </c>
       <c r="I1" s="15" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
-        <v>112</v>
-      </c>
-      <c r="B2" s="49" t="s">
-        <v>67</v>
+      <c r="A2" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>64</v>
       </c>
       <c r="C2" s="13">
         <v>1</v>
@@ -1571,20 +1555,20 @@
         <v>13</v>
       </c>
       <c r="E2" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="13" t="s">
         <v>61</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>64</v>
       </c>
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
       <c r="I2" s="13" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="50"/>
-      <c r="B3" s="50"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
       <c r="C3" s="14">
         <v>2</v>
       </c>
@@ -1592,18 +1576,18 @@
         <v>14</v>
       </c>
       <c r="E3" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="14" t="s">
         <v>62</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>65</v>
       </c>
       <c r="G3" s="14"/>
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
     </row>
     <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="50"/>
-      <c r="B4" s="50"/>
+      <c r="A4" s="35"/>
+      <c r="B4" s="35"/>
       <c r="C4" s="13">
         <v>3</v>
       </c>
@@ -1611,22 +1595,22 @@
         <v>19</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G4" s="13"/>
       <c r="H4" s="13" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="50"/>
-      <c r="B5" s="50"/>
+      <c r="A5" s="35"/>
+      <c r="B5" s="35"/>
       <c r="C5" s="14">
         <v>4</v>
       </c>
@@ -1634,22 +1618,22 @@
         <v>15</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G5" s="14"/>
       <c r="H5" s="14" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="50"/>
-      <c r="B6" s="50"/>
+      <c r="A6" s="35"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="13">
         <v>5</v>
       </c>
@@ -1657,22 +1641,22 @@
         <v>16</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G6" s="13"/>
       <c r="H6" s="13" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="50"/>
-      <c r="B7" s="50"/>
+      <c r="A7" s="35"/>
+      <c r="B7" s="35"/>
       <c r="C7" s="14">
         <v>6</v>
       </c>
@@ -1680,22 +1664,22 @@
         <v>17</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G7" s="14"/>
       <c r="H7" s="14" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="50"/>
-      <c r="B8" s="50"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="35"/>
       <c r="C8" s="13">
         <v>7</v>
       </c>
@@ -1703,105 +1687,105 @@
         <v>18</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G8" s="13"/>
       <c r="H8" s="13" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="50"/>
-      <c r="B9" s="50"/>
+      <c r="A9" s="35"/>
+      <c r="B9" s="35"/>
       <c r="C9" s="14">
         <v>8</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G9" s="14"/>
       <c r="H9" s="14" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="50"/>
-      <c r="B10" s="50"/>
+      <c r="A10" s="35"/>
+      <c r="B10" s="35"/>
       <c r="C10" s="13">
         <v>9</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G10" s="13"/>
       <c r="H10" s="13" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="I10" s="13" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="50"/>
-      <c r="B11" s="50"/>
+      <c r="A11" s="35"/>
+      <c r="B11" s="35"/>
       <c r="C11" s="14">
         <v>10</v>
       </c>
-      <c r="D11" s="40" t="s">
-        <v>68</v>
-      </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="42"/>
+      <c r="D11" s="51" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="53"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="51"/>
-      <c r="B12" s="51"/>
+      <c r="A12" s="36"/>
+      <c r="B12" s="36"/>
       <c r="C12" s="13">
         <v>11</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>69</v>
+        <v>20</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="58" t="s">
-        <v>113</v>
-      </c>
-      <c r="B13" s="58" t="s">
-        <v>76</v>
+      <c r="A13" s="43" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" s="43" t="s">
+        <v>70</v>
       </c>
       <c r="C13" s="21">
         <v>12</v>
@@ -1810,69 +1794,69 @@
         <v>22</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="G13" s="21"/>
       <c r="H13" s="21"/>
       <c r="I13" s="21"/>
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="59"/>
-      <c r="B14" s="59"/>
+      <c r="A14" s="44"/>
+      <c r="B14" s="44"/>
       <c r="C14" s="22">
         <v>13</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F14" s="22" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="G14" s="22"/>
       <c r="H14" s="22"/>
       <c r="I14" s="22"/>
     </row>
     <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="59"/>
-      <c r="B15" s="60"/>
+      <c r="A15" s="44"/>
+      <c r="B15" s="66"/>
       <c r="C15" s="21">
         <v>14</v>
       </c>
       <c r="D15" s="21" t="s">
-        <v>71</v>
+        <v>21</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="F15" s="21" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G15" s="21"/>
       <c r="H15" s="21"/>
       <c r="I15" s="21"/>
     </row>
     <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
-      <c r="B16" s="33" t="s">
-        <v>80</v>
+      <c r="A16" s="30"/>
+      <c r="B16" s="95" t="s">
+        <v>74</v>
       </c>
       <c r="C16" s="19">
         <v>15</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="G16" s="19"/>
       <c r="H16" s="19"/>
@@ -1880,20 +1864,18 @@
     </row>
     <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="27"/>
-      <c r="B17" s="28" t="s">
-        <v>82</v>
-      </c>
+      <c r="B17" s="96"/>
       <c r="C17" s="18">
         <v>16</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>130</v>
+        <v>108</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F17" s="18" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="G17" s="18"/>
       <c r="H17" s="18"/>
@@ -1905,75 +1887,75 @@
       <c r="C18" s="24">
         <v>17</v>
       </c>
-      <c r="D18" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="E18" s="44"/>
-      <c r="F18" s="44"/>
-      <c r="G18" s="44"/>
-      <c r="H18" s="44"/>
-      <c r="I18" s="45"/>
+      <c r="D18" s="54" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" s="55"/>
+      <c r="F18" s="55"/>
+      <c r="G18" s="55"/>
+      <c r="H18" s="55"/>
+      <c r="I18" s="56"/>
     </row>
     <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="67" t="s">
-        <v>114</v>
-      </c>
-      <c r="B19" s="55" t="s">
-        <v>85</v>
-      </c>
-      <c r="C19" s="30">
+      <c r="A19" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="B19" s="63" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="28">
         <v>18</v>
       </c>
-      <c r="D19" s="30" t="s">
-        <v>122</v>
-      </c>
-      <c r="E19" s="30" t="s">
-        <v>125</v>
-      </c>
-      <c r="F19" s="30" t="s">
-        <v>75</v>
-      </c>
-      <c r="G19" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="H19" s="30"/>
-      <c r="I19" s="30"/>
+      <c r="D19" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="E19" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="F19" s="28" t="s">
+        <v>69</v>
+      </c>
+      <c r="G19" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
     </row>
     <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="68"/>
-      <c r="B20" s="56"/>
-      <c r="C20" s="31">
+      <c r="A20" s="41"/>
+      <c r="B20" s="64"/>
+      <c r="C20" s="29">
         <v>19</v>
       </c>
-      <c r="D20" s="52" t="s">
-        <v>68</v>
-      </c>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
-      <c r="G20" s="53"/>
-      <c r="H20" s="53"/>
-      <c r="I20" s="54"/>
+      <c r="D20" s="60" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" s="61"/>
+      <c r="F20" s="61"/>
+      <c r="G20" s="61"/>
+      <c r="H20" s="61"/>
+      <c r="I20" s="62"/>
     </row>
     <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="69"/>
-      <c r="B21" s="57"/>
-      <c r="C21" s="30">
+      <c r="A21" s="42"/>
+      <c r="B21" s="65"/>
+      <c r="C21" s="28">
         <v>20</v>
       </c>
-      <c r="D21" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="E21" s="30" t="s">
-        <v>109</v>
-      </c>
-      <c r="F21" s="30" t="s">
-        <v>58</v>
-      </c>
-      <c r="G21" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="H21" s="30"/>
-      <c r="I21" s="30"/>
+      <c r="D21" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="E21" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="F21" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="G21" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
     </row>
     <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="27"/>
@@ -1981,21 +1963,21 @@
       <c r="C22" s="24">
         <v>21</v>
       </c>
-      <c r="D22" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="E22" s="44"/>
-      <c r="F22" s="44"/>
-      <c r="G22" s="44"/>
-      <c r="H22" s="44"/>
-      <c r="I22" s="45"/>
+      <c r="D22" s="54" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" s="55"/>
+      <c r="F22" s="55"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="55"/>
+      <c r="I22" s="56"/>
     </row>
     <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="64" t="s">
-        <v>115</v>
-      </c>
-      <c r="B23" s="34" t="s">
-        <v>84</v>
+      <c r="A23" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="B23" s="45" t="s">
+        <v>76</v>
       </c>
       <c r="C23" s="25">
         <v>22</v>
@@ -2004,70 +1986,64 @@
         <v>2</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="F23" s="25" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="G23" s="25" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="H23" s="25"/>
       <c r="I23" s="25"/>
     </row>
     <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="65"/>
-      <c r="B24" s="35"/>
+      <c r="A24" s="38"/>
+      <c r="B24" s="46"/>
       <c r="C24" s="26">
         <v>23</v>
       </c>
-      <c r="D24" s="26" t="s">
-        <v>89</v>
-      </c>
-      <c r="E24" s="26" t="s">
-        <v>125</v>
-      </c>
-      <c r="F24" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="G24" s="26" t="s">
-        <v>100</v>
-      </c>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
+      <c r="D24" s="97" t="s">
+        <v>65</v>
+      </c>
+      <c r="E24" s="98"/>
+      <c r="F24" s="98"/>
+      <c r="G24" s="98"/>
+      <c r="H24" s="98"/>
+      <c r="I24" s="99"/>
     </row>
     <row r="25" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="65"/>
-      <c r="B25" s="35"/>
+      <c r="A25" s="38"/>
+      <c r="B25" s="46"/>
       <c r="C25" s="25">
         <v>24</v>
       </c>
-      <c r="D25" s="46" t="s">
-        <v>68</v>
-      </c>
-      <c r="E25" s="47"/>
-      <c r="F25" s="47"/>
-      <c r="G25" s="47"/>
-      <c r="H25" s="47"/>
-      <c r="I25" s="48"/>
+      <c r="D25" s="57" t="s">
+        <v>65</v>
+      </c>
+      <c r="E25" s="58"/>
+      <c r="F25" s="58"/>
+      <c r="G25" s="58"/>
+      <c r="H25" s="58"/>
+      <c r="I25" s="59"/>
     </row>
     <row r="26" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="66"/>
-      <c r="B26" s="36"/>
+      <c r="A26" s="39"/>
+      <c r="B26" s="47"/>
       <c r="C26" s="26">
         <v>25</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>86</v>
+        <v>1</v>
       </c>
       <c r="E26" s="26" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="F26" s="26" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="G26" s="26" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="H26" s="26"/>
       <c r="I26" s="26"/>
@@ -2078,21 +2054,21 @@
       <c r="C27" s="24">
         <v>26</v>
       </c>
-      <c r="D27" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="E27" s="44"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="44"/>
-      <c r="H27" s="44"/>
-      <c r="I27" s="45"/>
+      <c r="D27" s="54" t="s">
+        <v>65</v>
+      </c>
+      <c r="E27" s="55"/>
+      <c r="F27" s="55"/>
+      <c r="G27" s="55"/>
+      <c r="H27" s="55"/>
+      <c r="I27" s="56"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="61" t="s">
-        <v>116</v>
-      </c>
-      <c r="B28" s="37" t="s">
-        <v>77</v>
+      <c r="A28" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="B28" s="48" t="s">
+        <v>71</v>
       </c>
       <c r="C28" s="16">
         <v>27</v>
@@ -2102,128 +2078,113 @@
       </c>
       <c r="E28" s="16"/>
       <c r="F28" s="16" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="G28" s="16" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="H28" s="16"/>
       <c r="I28" s="16"/>
     </row>
     <row r="29" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="62"/>
-      <c r="B29" s="38"/>
+      <c r="A29" s="32"/>
+      <c r="B29" s="49"/>
       <c r="C29" s="17">
         <v>28</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="E29" s="17"/>
       <c r="F29" s="17" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="G29" s="17" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="H29" s="17"/>
       <c r="I29" s="17"/>
     </row>
     <row r="30" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="62"/>
-      <c r="B30" s="38"/>
+      <c r="A30" s="32"/>
+      <c r="B30" s="49"/>
       <c r="C30" s="16">
         <v>29</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="E30" s="16"/>
       <c r="F30" s="16" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="G30" s="16" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="H30" s="16"/>
       <c r="I30" s="16"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="62"/>
-      <c r="B31" s="38"/>
+      <c r="A31" s="32"/>
+      <c r="B31" s="49"/>
       <c r="C31" s="17">
         <v>30</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>125</v>
+        <v>103</v>
       </c>
       <c r="F31" s="17" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="G31" s="17" t="s">
-        <v>105</v>
+        <v>123</v>
       </c>
       <c r="H31" s="17"/>
       <c r="I31" s="17"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="63"/>
-      <c r="B32" s="39"/>
+      <c r="A32" s="33"/>
+      <c r="B32" s="50"/>
       <c r="C32" s="16">
         <v>31</v>
       </c>
       <c r="D32" s="16" t="s">
-        <v>81</v>
+        <v>3</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F32" s="16" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="G32" s="16" t="s">
-        <v>106</v>
+        <v>124</v>
       </c>
       <c r="H32" s="16"/>
       <c r="I32" s="16"/>
     </row>
     <row r="33" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="27"/>
-      <c r="B33" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="C33" s="18">
+      <c r="B33" s="23"/>
+      <c r="C33" s="24">
         <v>32</v>
       </c>
-      <c r="D33" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="E33" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="F33" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="G33" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="H33" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="I33" s="18" t="s">
-        <v>97</v>
-      </c>
+      <c r="D33" s="54" t="s">
+        <v>65</v>
+      </c>
+      <c r="E33" s="55"/>
+      <c r="F33" s="55"/>
+      <c r="G33" s="55"/>
+      <c r="H33" s="55"/>
+      <c r="I33" s="56"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="A28:A32"/>
-    <mergeCell ref="A2:A12"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="A13:A15"/>
+  <mergeCells count="19">
+    <mergeCell ref="D33:I33"/>
+    <mergeCell ref="D24:I24"/>
     <mergeCell ref="B23:B26"/>
     <mergeCell ref="B28:B32"/>
     <mergeCell ref="D11:I11"/>
@@ -2235,6 +2196,12 @@
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B13:B15"/>
     <mergeCell ref="D18:I18"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A28:A32"/>
+    <mergeCell ref="A2:A12"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="A13:A15"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2247,7 +2214,7 @@
   <dimension ref="A1:S34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+      <selection activeCell="G20" sqref="G20:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2261,40 +2228,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="87" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
+      <c r="A1" s="70" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
       <c r="I1" s="3"/>
-      <c r="K1" s="83" t="s">
+      <c r="K1" s="87" t="s">
         <v>47</v>
       </c>
-      <c r="L1" s="83"/>
-      <c r="M1" s="83"/>
+      <c r="L1" s="87"/>
+      <c r="M1" s="87"/>
       <c r="N1" s="3"/>
-      <c r="P1" s="91" t="s">
+      <c r="P1" s="82" t="s">
         <v>41</v>
       </c>
-      <c r="Q1" s="91"/>
-      <c r="R1" s="91"/>
+      <c r="Q1" s="82"/>
+      <c r="R1" s="82"/>
     </row>
     <row r="2" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="87" t="s">
+      <c r="A2" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="87"/>
-      <c r="C2" s="87"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="87"/>
-      <c r="H2" s="87"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
       <c r="I2" s="3"/>
       <c r="K2" s="5" t="s">
         <v>48</v>
@@ -2304,9 +2271,9 @@
         <v>49</v>
       </c>
       <c r="N2" s="3"/>
-      <c r="P2" s="91"/>
-      <c r="Q2" s="91"/>
-      <c r="R2" s="91"/>
+      <c r="P2" s="82"/>
+      <c r="Q2" s="82"/>
+      <c r="R2" s="82"/>
     </row>
     <row r="3" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -2334,94 +2301,94 @@
         <v>8</v>
       </c>
       <c r="I3" s="3"/>
-      <c r="K3" s="70" t="s">
+      <c r="K3" s="81" t="s">
+        <v>111</v>
+      </c>
+      <c r="L3" s="81"/>
+      <c r="M3" s="81"/>
+      <c r="N3" s="3"/>
+      <c r="P3" s="80" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q3" s="84" t="s">
+        <v>27</v>
+      </c>
+      <c r="R3" s="80" t="s">
         <v>29</v>
       </c>
-      <c r="L3" s="70"/>
-      <c r="M3" s="70"/>
-      <c r="N3" s="3"/>
-      <c r="P3" s="92" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q3" s="74" t="s">
-        <v>27</v>
-      </c>
-      <c r="R3" s="92" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="4" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="79" t="s">
+      <c r="A4" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="79" t="s">
+      <c r="B4" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="79" t="s">
+      <c r="C4" s="73" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="79" t="s">
+      <c r="D4" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="77" t="s">
+      <c r="E4" s="74" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="77" t="s">
+      <c r="F4" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="77" t="s">
+      <c r="G4" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="79" t="s">
-        <v>119</v>
+      <c r="H4" s="73" t="s">
+        <v>99</v>
       </c>
       <c r="I4" s="3"/>
-      <c r="K4" s="93" t="s">
+      <c r="K4" s="78" t="s">
         <v>46</v>
       </c>
       <c r="L4" s="11">
         <v>1</v>
       </c>
-      <c r="M4" s="94" t="s">
+      <c r="M4" s="79" t="s">
         <v>50</v>
       </c>
       <c r="N4" s="3"/>
-      <c r="P4" s="92"/>
-      <c r="Q4" s="74"/>
-      <c r="R4" s="92"/>
+      <c r="P4" s="80"/>
+      <c r="Q4" s="84"/>
+      <c r="R4" s="80"/>
     </row>
     <row r="5" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="79"/>
-      <c r="B5" s="79"/>
-      <c r="C5" s="79"/>
-      <c r="D5" s="79"/>
-      <c r="E5" s="78"/>
-      <c r="F5" s="78"/>
-      <c r="G5" s="78"/>
-      <c r="H5" s="79"/>
+      <c r="A5" s="73"/>
+      <c r="B5" s="73"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="73"/>
       <c r="I5" s="3"/>
-      <c r="K5" s="93"/>
+      <c r="K5" s="78"/>
       <c r="L5" s="12">
-        <v>3</v>
-      </c>
-      <c r="M5" s="94"/>
+        <v>2</v>
+      </c>
+      <c r="M5" s="79"/>
       <c r="N5" s="3"/>
-      <c r="P5" s="92"/>
-      <c r="Q5" s="74"/>
-      <c r="R5" s="92"/>
+      <c r="P5" s="80"/>
+      <c r="Q5" s="84"/>
+      <c r="R5" s="80"/>
     </row>
     <row r="6" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I6" s="3"/>
-      <c r="K6" s="70" t="s">
-        <v>96</v>
-      </c>
-      <c r="L6" s="70"/>
-      <c r="M6" s="70"/>
+      <c r="K6" s="81" t="s">
+        <v>45</v>
+      </c>
+      <c r="L6" s="81"/>
+      <c r="M6" s="81"/>
       <c r="N6" s="3"/>
       <c r="P6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="Q6" s="74"/>
+      <c r="Q6" s="84"/>
       <c r="R6" s="7" t="s">
         <v>26</v>
       </c>
@@ -2452,115 +2419,101 @@
         <v>16</v>
       </c>
       <c r="I7" s="3"/>
-      <c r="K7" s="93" t="s">
+      <c r="K7" s="78" t="s">
         <v>46</v>
       </c>
       <c r="L7" s="11">
         <v>2</v>
       </c>
-      <c r="M7" s="94" t="s">
+      <c r="M7" s="79" t="s">
         <v>50</v>
       </c>
       <c r="N7" s="3"/>
     </row>
     <row r="8" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="79" t="s">
-        <v>120</v>
-      </c>
-      <c r="B8" s="81"/>
-      <c r="C8" s="79" t="s">
+      <c r="A8" s="73" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" s="69"/>
+      <c r="C8" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="80" t="s">
+      <c r="D8" s="94" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="80" t="s">
-        <v>124</v>
-      </c>
-      <c r="F8" s="80" t="s">
+      <c r="E8" s="94" t="s">
+        <v>102</v>
+      </c>
+      <c r="F8" s="94" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="75" t="s">
-        <v>128</v>
-      </c>
-      <c r="H8" s="75" t="s">
-        <v>127</v>
+      <c r="G8" s="92" t="s">
+        <v>106</v>
+      </c>
+      <c r="H8" s="92" t="s">
+        <v>105</v>
       </c>
       <c r="I8" s="3"/>
-      <c r="K8" s="93"/>
+      <c r="K8" s="78"/>
       <c r="L8" s="12">
-        <v>2</v>
-      </c>
-      <c r="M8" s="94"/>
+        <v>1</v>
+      </c>
+      <c r="M8" s="79"/>
       <c r="N8" s="3"/>
-      <c r="P8" s="92" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q8" s="74" t="s">
+      <c r="P8" s="80" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q8" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="R8" s="92" t="s">
+      <c r="R8" s="80" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="79"/>
-      <c r="B9" s="81"/>
-      <c r="C9" s="79"/>
-      <c r="D9" s="80"/>
-      <c r="E9" s="80"/>
-      <c r="F9" s="80"/>
-      <c r="G9" s="76"/>
-      <c r="H9" s="76"/>
+      <c r="A9" s="73"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="94"/>
+      <c r="E9" s="94"/>
+      <c r="F9" s="94"/>
+      <c r="G9" s="93"/>
+      <c r="H9" s="93"/>
       <c r="I9" s="3"/>
-      <c r="K9" s="70" t="s">
+      <c r="K9" s="81" t="s">
         <v>44</v>
       </c>
-      <c r="L9" s="70"/>
-      <c r="M9" s="70"/>
+      <c r="L9" s="81"/>
+      <c r="M9" s="81"/>
       <c r="N9" s="3"/>
-      <c r="P9" s="92"/>
-      <c r="Q9" s="74"/>
-      <c r="R9" s="92"/>
+      <c r="P9" s="80"/>
+      <c r="Q9" s="84"/>
+      <c r="R9" s="80"/>
     </row>
     <row r="10" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I10" s="3"/>
-      <c r="K10" s="93" t="s">
-        <v>46</v>
-      </c>
-      <c r="L10" s="11">
-        <v>3</v>
-      </c>
-      <c r="M10" s="94" t="s">
-        <v>50</v>
-      </c>
       <c r="N10" s="3"/>
-      <c r="P10" s="92"/>
-      <c r="Q10" s="74"/>
-      <c r="R10" s="92"/>
+      <c r="P10" s="80"/>
+      <c r="Q10" s="84"/>
+      <c r="R10" s="80"/>
     </row>
     <row r="11" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="87" t="s">
+      <c r="A11" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="87"/>
-      <c r="C11" s="87"/>
-      <c r="D11" s="87"/>
-      <c r="E11" s="87"/>
-      <c r="F11" s="87"/>
-      <c r="G11" s="87"/>
-      <c r="H11" s="87"/>
+      <c r="B11" s="70"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="70"/>
+      <c r="H11" s="70"/>
       <c r="I11" s="3"/>
-      <c r="K11" s="93"/>
-      <c r="L11" s="12">
-        <v>1</v>
-      </c>
-      <c r="M11" s="94"/>
       <c r="N11" s="3"/>
       <c r="P11" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="Q11" s="74"/>
+      <c r="Q11" s="84"/>
       <c r="R11" s="7" t="s">
         <v>28</v>
       </c>
@@ -2591,28 +2544,23 @@
         <v>8</v>
       </c>
       <c r="I12" s="3"/>
-      <c r="K12" s="70" t="s">
-        <v>45</v>
-      </c>
-      <c r="L12" s="70"/>
-      <c r="M12" s="70"/>
       <c r="N12" s="3"/>
     </row>
     <row r="13" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="77" t="s">
+      <c r="A13" s="74" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="79" t="s">
+      <c r="B13" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="80" t="s">
+      <c r="C13" s="94" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="81"/>
-      <c r="E13" s="81"/>
-      <c r="F13" s="81"/>
-      <c r="G13" s="81"/>
-      <c r="H13" s="82" t="s">
+      <c r="D13" s="69"/>
+      <c r="E13" s="69"/>
+      <c r="F13" s="69"/>
+      <c r="G13" s="69"/>
+      <c r="H13" s="85" t="s">
         <v>23</v>
       </c>
       <c r="I13" s="3"/>
@@ -2627,14 +2575,14 @@
       <c r="R13" s="2"/>
     </row>
     <row r="14" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="78"/>
-      <c r="B14" s="79"/>
-      <c r="C14" s="80"/>
-      <c r="D14" s="81"/>
-      <c r="E14" s="81"/>
-      <c r="F14" s="81"/>
-      <c r="G14" s="81"/>
-      <c r="H14" s="82"/>
+      <c r="A14" s="75"/>
+      <c r="B14" s="73"/>
+      <c r="C14" s="94"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="69"/>
+      <c r="G14" s="69"/>
+      <c r="H14" s="86"/>
       <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2647,80 +2595,80 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="3"/>
-      <c r="K15" s="91" t="s">
+      <c r="K15" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="L15" s="91"/>
-      <c r="M15" s="91"/>
-      <c r="N15" s="91"/>
-      <c r="O15" s="91"/>
-      <c r="P15" s="91"/>
-      <c r="Q15" s="91"/>
+      <c r="L15" s="82"/>
+      <c r="M15" s="82"/>
+      <c r="N15" s="82"/>
+      <c r="O15" s="82"/>
+      <c r="P15" s="82"/>
+      <c r="Q15" s="82"/>
     </row>
     <row r="16" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I16" s="3"/>
-      <c r="K16" s="70" t="s">
-        <v>54</v>
-      </c>
-      <c r="L16" s="74" t="s">
+      <c r="K16" s="81" t="s">
+        <v>114</v>
+      </c>
+      <c r="L16" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="M16" s="70" t="s">
+      <c r="M16" s="81" t="s">
         <v>39</v>
       </c>
-      <c r="O16" s="70" t="s">
+      <c r="O16" s="81" t="s">
         <v>39</v>
       </c>
-      <c r="P16" s="74" t="s">
+      <c r="P16" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="Q16" s="70" t="s">
+      <c r="Q16" s="81" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="87" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17" s="87"/>
-      <c r="C17" s="87"/>
-      <c r="D17" s="87"/>
-      <c r="E17" s="87"/>
-      <c r="F17" s="87"/>
-      <c r="G17" s="87"/>
-      <c r="H17" s="87"/>
+      <c r="A17" s="70" t="s">
+        <v>113</v>
+      </c>
+      <c r="B17" s="70"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="70"/>
+      <c r="E17" s="70"/>
+      <c r="F17" s="70"/>
+      <c r="G17" s="70"/>
+      <c r="H17" s="70"/>
       <c r="I17" s="3"/>
-      <c r="K17" s="71"/>
-      <c r="L17" s="74"/>
-      <c r="M17" s="70"/>
-      <c r="O17" s="70"/>
-      <c r="P17" s="74"/>
-      <c r="Q17" s="70"/>
+      <c r="K17" s="83"/>
+      <c r="L17" s="84"/>
+      <c r="M17" s="81"/>
+      <c r="O17" s="81"/>
+      <c r="P17" s="84"/>
+      <c r="Q17" s="81"/>
     </row>
     <row r="18" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="87" t="s">
+      <c r="A18" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="87"/>
-      <c r="C18" s="87"/>
-      <c r="D18" s="87"/>
-      <c r="E18" s="87"/>
-      <c r="F18" s="87"/>
-      <c r="G18" s="87"/>
-      <c r="H18" s="87"/>
+      <c r="B18" s="70"/>
+      <c r="C18" s="70"/>
+      <c r="D18" s="70"/>
+      <c r="E18" s="70"/>
+      <c r="F18" s="70"/>
+      <c r="G18" s="70"/>
+      <c r="H18" s="70"/>
       <c r="I18" s="3"/>
-      <c r="K18" s="72" t="s">
+      <c r="K18" s="85" t="s">
         <v>9</v>
       </c>
-      <c r="L18" s="74"/>
-      <c r="M18" s="72" t="s">
+      <c r="L18" s="84"/>
+      <c r="M18" s="85" t="s">
         <v>38</v>
       </c>
-      <c r="O18" s="72" t="s">
+      <c r="O18" s="85" t="s">
         <v>43</v>
       </c>
-      <c r="P18" s="74"/>
-      <c r="Q18" s="72" t="s">
+      <c r="P18" s="84"/>
+      <c r="Q18" s="85" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2750,66 +2698,66 @@
         <v>8</v>
       </c>
       <c r="I19" s="3"/>
-      <c r="K19" s="73"/>
-      <c r="L19" s="74"/>
-      <c r="M19" s="73"/>
-      <c r="O19" s="73"/>
-      <c r="P19" s="74"/>
-      <c r="Q19" s="73"/>
+      <c r="K19" s="86"/>
+      <c r="L19" s="84"/>
+      <c r="M19" s="86"/>
+      <c r="O19" s="86"/>
+      <c r="P19" s="84"/>
+      <c r="Q19" s="86"/>
     </row>
     <row r="20" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="81"/>
-      <c r="B20" s="88" t="s">
-        <v>122</v>
-      </c>
-      <c r="C20" s="82"/>
-      <c r="D20" s="89" t="s">
-        <v>110</v>
-      </c>
-      <c r="E20" s="81"/>
-      <c r="F20" s="86" t="s">
+      <c r="A20" s="69"/>
+      <c r="B20" s="89" t="s">
+        <v>101</v>
+      </c>
+      <c r="C20" s="72"/>
+      <c r="D20" s="90" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" s="69"/>
+      <c r="F20" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="G20" s="86" t="s">
-        <v>126</v>
-      </c>
-      <c r="H20" s="86"/>
+      <c r="G20" s="76" t="s">
+        <v>104</v>
+      </c>
+      <c r="H20" s="76"/>
       <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="81"/>
-      <c r="B21" s="88"/>
-      <c r="C21" s="82"/>
-      <c r="D21" s="90"/>
-      <c r="E21" s="81"/>
-      <c r="F21" s="86"/>
-      <c r="G21" s="86"/>
-      <c r="H21" s="86"/>
+      <c r="A21" s="69"/>
+      <c r="B21" s="89"/>
+      <c r="C21" s="72"/>
+      <c r="D21" s="91"/>
+      <c r="E21" s="69"/>
+      <c r="F21" s="76"/>
+      <c r="G21" s="76"/>
+      <c r="H21" s="76"/>
       <c r="I21" s="3"/>
-      <c r="L21" s="74" t="s">
+      <c r="L21" s="84" t="s">
         <v>27</v>
       </c>
-      <c r="P21" s="74" t="s">
+      <c r="P21" s="84" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F22" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="I22" s="3"/>
-      <c r="K22" s="70" t="s">
+      <c r="K22" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="L22" s="74"/>
-      <c r="M22" s="70" t="s">
+      <c r="L22" s="84"/>
+      <c r="M22" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="O22" s="70" t="s">
+      <c r="O22" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="P22" s="74"/>
-      <c r="Q22" s="70" t="s">
+      <c r="P22" s="84"/>
+      <c r="Q22" s="81" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2839,68 +2787,68 @@
         <v>16</v>
       </c>
       <c r="I23" s="3"/>
-      <c r="K23" s="71"/>
-      <c r="L23" s="74"/>
-      <c r="M23" s="71"/>
-      <c r="O23" s="71"/>
-      <c r="P23" s="74"/>
-      <c r="Q23" s="71"/>
+      <c r="K23" s="83"/>
+      <c r="L23" s="84"/>
+      <c r="M23" s="83"/>
+      <c r="O23" s="83"/>
+      <c r="P23" s="84"/>
+      <c r="Q23" s="83"/>
     </row>
     <row r="24" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="86" t="s">
+      <c r="A24" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="B24" s="81"/>
-      <c r="C24" s="84" t="s">
+      <c r="B24" s="69"/>
+      <c r="C24" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="D24" s="84" t="s">
+      <c r="D24" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="E24" s="84" t="s">
+      <c r="E24" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="F24" s="84" t="s">
+      <c r="F24" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="G24" s="84" t="s">
+      <c r="G24" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="H24" s="85" t="s">
+      <c r="H24" s="88" t="s">
         <v>10</v>
       </c>
       <c r="I24" s="3"/>
-      <c r="K24" s="72" t="s">
-        <v>9</v>
-      </c>
-      <c r="L24" s="74"/>
-      <c r="M24" s="72" t="s">
+      <c r="K24" s="85" t="s">
+        <v>23</v>
+      </c>
+      <c r="L24" s="84"/>
+      <c r="M24" s="85" t="s">
         <v>38</v>
       </c>
-      <c r="O24" s="72" t="s">
+      <c r="O24" s="85" t="s">
         <v>43</v>
       </c>
-      <c r="P24" s="74"/>
-      <c r="Q24" s="72" t="s">
+      <c r="P24" s="84"/>
+      <c r="Q24" s="85" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="86"/>
-      <c r="B25" s="81"/>
-      <c r="C25" s="84"/>
-      <c r="D25" s="84"/>
-      <c r="E25" s="84"/>
-      <c r="F25" s="84"/>
-      <c r="G25" s="84"/>
-      <c r="H25" s="85"/>
+      <c r="A25" s="76"/>
+      <c r="B25" s="69"/>
+      <c r="C25" s="77"/>
+      <c r="D25" s="77"/>
+      <c r="E25" s="77"/>
+      <c r="F25" s="77"/>
+      <c r="G25" s="77"/>
+      <c r="H25" s="88"/>
       <c r="I25" s="3"/>
-      <c r="K25" s="73"/>
-      <c r="L25" s="74"/>
-      <c r="M25" s="73"/>
-      <c r="O25" s="73"/>
-      <c r="P25" s="74"/>
-      <c r="Q25" s="73"/>
+      <c r="K25" s="86"/>
+      <c r="L25" s="84"/>
+      <c r="M25" s="86"/>
+      <c r="O25" s="86"/>
+      <c r="P25" s="84"/>
+      <c r="Q25" s="86"/>
     </row>
     <row r="26" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I26" s="3"/>
@@ -2912,16 +2860,16 @@
       <c r="Q26" s="4"/>
     </row>
     <row r="27" spans="1:18" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="87" t="s">
+      <c r="A27" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="87"/>
-      <c r="C27" s="87"/>
-      <c r="D27" s="87"/>
-      <c r="E27" s="87"/>
-      <c r="F27" s="87"/>
-      <c r="G27" s="87"/>
-      <c r="H27" s="87"/>
+      <c r="B27" s="70"/>
+      <c r="C27" s="70"/>
+      <c r="D27" s="70"/>
+      <c r="E27" s="70"/>
+      <c r="F27" s="70"/>
+      <c r="G27" s="70"/>
+      <c r="H27" s="70"/>
       <c r="I27" s="3"/>
       <c r="J27" s="10"/>
       <c r="K27" s="2"/>
@@ -2959,138 +2907,205 @@
         <v>8</v>
       </c>
       <c r="I28" s="3"/>
-      <c r="K28" s="95" t="s">
+      <c r="K28" s="71" t="s">
         <v>30</v>
       </c>
-      <c r="L28" s="95"/>
-      <c r="M28" s="95"/>
-      <c r="N28" s="95"/>
-      <c r="O28" s="95"/>
-      <c r="P28" s="95"/>
-      <c r="Q28" s="95"/>
-      <c r="R28" s="95"/>
+      <c r="L28" s="71"/>
+      <c r="M28" s="71"/>
+      <c r="N28" s="71"/>
+      <c r="O28" s="71"/>
+      <c r="P28" s="71"/>
+      <c r="Q28" s="71"/>
+      <c r="R28" s="71"/>
     </row>
     <row r="29" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="82" t="s">
-        <v>131</v>
-      </c>
-      <c r="B29" s="81"/>
-      <c r="C29" s="86" t="s">
+      <c r="A29" s="72" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29" s="69"/>
+      <c r="C29" s="76" t="s">
         <v>24</v>
       </c>
-      <c r="D29" s="81"/>
-      <c r="E29" s="84" t="s">
+      <c r="D29" s="69"/>
+      <c r="E29" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="F29" s="81"/>
-      <c r="G29" s="81"/>
-      <c r="H29" s="82" t="s">
+      <c r="F29" s="69"/>
+      <c r="G29" s="69"/>
+      <c r="H29" s="85" t="s">
         <v>9</v>
       </c>
       <c r="I29" s="3"/>
       <c r="K29" s="20">
         <v>1</v>
       </c>
-      <c r="L29" s="96" t="s">
+      <c r="L29" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="M29" s="96"/>
-      <c r="N29" s="96"/>
-      <c r="O29" s="96"/>
-      <c r="P29" s="96"/>
-      <c r="Q29" s="96"/>
-      <c r="R29" s="96"/>
+      <c r="M29" s="68"/>
+      <c r="N29" s="68"/>
+      <c r="O29" s="68"/>
+      <c r="P29" s="68"/>
+      <c r="Q29" s="68"/>
+      <c r="R29" s="68"/>
     </row>
     <row r="30" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="82"/>
-      <c r="B30" s="81"/>
-      <c r="C30" s="86"/>
-      <c r="D30" s="81"/>
-      <c r="E30" s="84"/>
-      <c r="F30" s="81"/>
-      <c r="G30" s="81"/>
-      <c r="H30" s="82"/>
+      <c r="A30" s="72"/>
+      <c r="B30" s="69"/>
+      <c r="C30" s="76"/>
+      <c r="D30" s="69"/>
+      <c r="E30" s="77"/>
+      <c r="F30" s="69"/>
+      <c r="G30" s="69"/>
+      <c r="H30" s="86"/>
       <c r="I30" s="3"/>
       <c r="K30" s="8">
         <v>2</v>
       </c>
-      <c r="L30" s="97" t="s">
+      <c r="L30" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="M30" s="97"/>
-      <c r="N30" s="97"/>
-      <c r="O30" s="97"/>
-      <c r="P30" s="97"/>
-      <c r="Q30" s="97"/>
-      <c r="R30" s="97"/>
+      <c r="M30" s="67"/>
+      <c r="N30" s="67"/>
+      <c r="O30" s="67"/>
+      <c r="P30" s="67"/>
+      <c r="Q30" s="67"/>
+      <c r="R30" s="67"/>
     </row>
     <row r="31" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I31" s="3"/>
       <c r="K31" s="20">
         <v>3</v>
       </c>
-      <c r="L31" s="96" t="s">
+      <c r="L31" s="68" t="s">
         <v>51</v>
       </c>
-      <c r="M31" s="96"/>
-      <c r="N31" s="96"/>
-      <c r="O31" s="96"/>
-      <c r="P31" s="96"/>
-      <c r="Q31" s="96"/>
-      <c r="R31" s="96"/>
+      <c r="M31" s="68"/>
+      <c r="N31" s="68"/>
+      <c r="O31" s="68"/>
+      <c r="P31" s="68"/>
+      <c r="Q31" s="68"/>
+      <c r="R31" s="68"/>
     </row>
     <row r="32" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I32" s="3"/>
       <c r="K32" s="8">
         <v>4</v>
       </c>
-      <c r="L32" s="97" t="s">
+      <c r="L32" s="67" t="s">
         <v>52</v>
       </c>
-      <c r="M32" s="97"/>
-      <c r="N32" s="97"/>
-      <c r="O32" s="97"/>
-      <c r="P32" s="97"/>
-      <c r="Q32" s="97"/>
-      <c r="R32" s="97"/>
+      <c r="M32" s="67"/>
+      <c r="N32" s="67"/>
+      <c r="O32" s="67"/>
+      <c r="P32" s="67"/>
+      <c r="Q32" s="67"/>
+      <c r="R32" s="67"/>
     </row>
     <row r="33" spans="9:18" x14ac:dyDescent="0.25">
       <c r="I33" s="3"/>
       <c r="K33" s="20">
         <v>5</v>
       </c>
-      <c r="L33" s="96" t="s">
-        <v>53</v>
-      </c>
-      <c r="M33" s="96"/>
-      <c r="N33" s="96"/>
-      <c r="O33" s="96"/>
-      <c r="P33" s="96"/>
-      <c r="Q33" s="96"/>
-      <c r="R33" s="96"/>
+      <c r="L33" s="68" t="s">
+        <v>110</v>
+      </c>
+      <c r="M33" s="68"/>
+      <c r="N33" s="68"/>
+      <c r="O33" s="68"/>
+      <c r="P33" s="68"/>
+      <c r="Q33" s="68"/>
+      <c r="R33" s="68"/>
     </row>
     <row r="34" spans="9:18" x14ac:dyDescent="0.25">
       <c r="I34" s="3"/>
-      <c r="K34" s="8">
-        <v>5</v>
-      </c>
-      <c r="L34" s="97" t="s">
-        <v>55</v>
-      </c>
-      <c r="M34" s="97"/>
-      <c r="N34" s="97"/>
-      <c r="O34" s="97"/>
-      <c r="P34" s="97"/>
-      <c r="Q34" s="97"/>
-      <c r="R34" s="97"/>
+      <c r="K34" s="8"/>
+      <c r="L34" s="67"/>
+      <c r="M34" s="67"/>
+      <c r="N34" s="67"/>
+      <c r="O34" s="67"/>
+      <c r="P34" s="67"/>
+      <c r="Q34" s="67"/>
+      <c r="R34" s="67"/>
     </row>
   </sheetData>
-  <mergeCells count="100">
-    <mergeCell ref="L32:R32"/>
-    <mergeCell ref="L33:R33"/>
-    <mergeCell ref="L34:R34"/>
-    <mergeCell ref="L29:R29"/>
-    <mergeCell ref="L30:R30"/>
+  <mergeCells count="97">
+    <mergeCell ref="Q22:Q23"/>
+    <mergeCell ref="O24:O25"/>
+    <mergeCell ref="Q24:Q25"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="Q18:Q19"/>
+    <mergeCell ref="L21:L25"/>
+    <mergeCell ref="P21:P25"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="O22:O23"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="P1:R2"/>
+    <mergeCell ref="K15:Q15"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="L16:L19"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="O16:O17"/>
+    <mergeCell ref="P16:P19"/>
+    <mergeCell ref="Q16:Q17"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="P8:P10"/>
+    <mergeCell ref="Q8:Q11"/>
+    <mergeCell ref="Q3:Q6"/>
+    <mergeCell ref="R8:R10"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="R3:R5"/>
+    <mergeCell ref="P3:P5"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="A11:H11"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
     <mergeCell ref="F29:F30"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:H2"/>
@@ -3107,85 +3122,11 @@
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="H4:H5"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="A11:H11"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="M10:M11"/>
-    <mergeCell ref="R3:R5"/>
-    <mergeCell ref="P3:P5"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="P1:R2"/>
-    <mergeCell ref="K15:Q15"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="L16:L19"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="O16:O17"/>
-    <mergeCell ref="P16:P19"/>
-    <mergeCell ref="Q16:Q17"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="P8:P10"/>
-    <mergeCell ref="Q8:Q11"/>
-    <mergeCell ref="Q3:Q6"/>
-    <mergeCell ref="R8:R10"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="A18:H18"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="Q22:Q23"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="O24:O25"/>
-    <mergeCell ref="Q24:Q25"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="Q18:Q19"/>
-    <mergeCell ref="L21:L25"/>
-    <mergeCell ref="P21:P25"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="M24:M25"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="O22:O23"/>
+    <mergeCell ref="L32:R32"/>
+    <mergeCell ref="L33:R33"/>
+    <mergeCell ref="L34:R34"/>
+    <mergeCell ref="L29:R29"/>
+    <mergeCell ref="L30:R30"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New layout for split
</commit_message>
<xml_diff>
--- a/Input List/Input List.xlsx
+++ b/Input List/Input List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\TechnicalDocumentation\Input List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F5BBD3D-9289-423C-9F5D-4856386DDA22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24181059-2C31-450E-8FAA-E8C56745C15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
+    <workbookView xWindow="-165" yWindow="-165" windowWidth="29130" windowHeight="15810" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
   </bookViews>
   <sheets>
     <sheet name="Input + Equipment" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="95">
   <si>
     <t>Input</t>
   </si>
@@ -100,9 +100,6 @@
   </si>
   <si>
     <t>Notes</t>
-  </si>
-  <si>
-    <t>Chad's IEM channels are stereo</t>
   </si>
   <si>
     <t>Channel</t>
@@ -262,24 +259,9 @@
     <t>Bluetooth Right</t>
   </si>
   <si>
-    <t>Kenzi IEM L</t>
-  </si>
-  <si>
-    <t>Kenzi IEM R</t>
-  </si>
-  <si>
-    <t>Paul IEM L</t>
-  </si>
-  <si>
-    <t>Paul IEM R</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Paul's IEM transmitter Port 1 does not work</t>
-  </si>
-  <si>
     <t>Colored cables = band vocals &amp; instruments</t>
   </si>
   <si>
@@ -301,21 +283,9 @@
     <t>Guitars, Bass, and Keys Snake</t>
   </si>
   <si>
-    <t>John IEM L</t>
-  </si>
-  <si>
-    <t>John IEM R</t>
-  </si>
-  <si>
     <t>Jessica Acstc</t>
   </si>
   <si>
-    <t>Jessica IEM L</t>
-  </si>
-  <si>
-    <t>Jessica IEM R</t>
-  </si>
-  <si>
     <t>Black cables = utility (PA and patching)</t>
   </si>
   <si>
@@ -325,16 +295,34 @@
     <t>Shure SM57</t>
   </si>
   <si>
-    <t>Chad IEM L</t>
-  </si>
-  <si>
-    <t>Chad IEM R</t>
-  </si>
-  <si>
     <t>Main Right</t>
   </si>
   <si>
     <t>Snake</t>
+  </si>
+  <si>
+    <t>Drum Snake outputs are used to extend splitter</t>
+  </si>
+  <si>
+    <t>Paul's IEM transmitter Port 1 does not work (capped)</t>
+  </si>
+  <si>
+    <t>Black patch cables in the box are not to be unplugged</t>
+  </si>
+  <si>
+    <t>Paul IEM</t>
+  </si>
+  <si>
+    <t>Chad IEM</t>
+  </si>
+  <si>
+    <t>Kenzi IEM</t>
+  </si>
+  <si>
+    <t>Jessica IEM</t>
+  </si>
+  <si>
+    <t>John IEM</t>
   </si>
 </sst>
 </file>
@@ -788,7 +776,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -827,149 +815,152 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1145,9 +1136,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1185,7 +1176,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1291,7 +1282,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1433,7 +1424,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1443,714 +1434,714 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18A11D25-D77D-4358-9E34-E04B11CA4C7B}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" style="58" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="22" width="7.28515625" customWidth="1"/>
+    <col min="1" max="1" width="8.81640625" customWidth="1"/>
+    <col min="2" max="2" width="7.54296875" customWidth="1"/>
+    <col min="3" max="3" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="35.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="22" width="7.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="74" t="s">
-        <v>98</v>
+        <v>21</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>86</v>
       </c>
       <c r="E1" s="22" t="s">
         <v>0</v>
       </c>
       <c r="F1" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="H1" s="22" t="s">
         <v>24</v>
-      </c>
-      <c r="H1" s="22" t="s">
-        <v>25</v>
       </c>
       <c r="I1" s="22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>32</v>
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>31</v>
       </c>
       <c r="C2" s="4">
         <v>1</v>
       </c>
-      <c r="D2" s="61">
+      <c r="D2" s="4">
         <v>1</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="36"/>
+      <c r="B3" s="36"/>
       <c r="C3" s="5">
         <v>2</v>
       </c>
-      <c r="D3" s="62">
+      <c r="D3" s="5">
         <v>2</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="28"/>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
       <c r="C4" s="4">
         <v>3</v>
       </c>
-      <c r="D4" s="61">
+      <c r="D4" s="4">
         <v>3</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
-      <c r="B5" s="28"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="36"/>
+      <c r="B5" s="36"/>
       <c r="C5" s="5">
         <v>4</v>
       </c>
-      <c r="D5" s="62">
+      <c r="D5" s="5">
         <v>4</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>12</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
-      <c r="B6" s="28"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="36"/>
+      <c r="B6" s="36"/>
       <c r="C6" s="4">
         <v>5</v>
       </c>
-      <c r="D6" s="61">
+      <c r="D6" s="4">
         <v>5</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
-      <c r="B7" s="28"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="36"/>
+      <c r="B7" s="36"/>
       <c r="C7" s="5">
         <v>6</v>
       </c>
-      <c r="D7" s="62">
+      <c r="D7" s="5">
         <v>6</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
-      <c r="B8" s="28"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="36"/>
+      <c r="B8" s="36"/>
       <c r="C8" s="4">
         <v>7</v>
       </c>
-      <c r="D8" s="61">
+      <c r="D8" s="4">
         <v>7</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
-      <c r="B9" s="28"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="36"/>
+      <c r="B9" s="36"/>
       <c r="C9" s="5">
         <v>8</v>
       </c>
-      <c r="D9" s="62">
+      <c r="D9" s="5">
         <v>8</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
-      <c r="B10" s="28"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="36"/>
+      <c r="B10" s="36"/>
       <c r="C10" s="4">
         <v>9</v>
       </c>
-      <c r="D10" s="61">
+      <c r="D10" s="4">
         <v>9</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
-      <c r="B11" s="28"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="36"/>
+      <c r="B11" s="36"/>
       <c r="C11" s="5">
         <v>10</v>
       </c>
-      <c r="D11" s="62">
+      <c r="D11" s="5">
         <v>10</v>
       </c>
-      <c r="E11" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="30"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
-      <c r="B12" s="28"/>
+      <c r="E11" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="36"/>
+      <c r="B12" s="36"/>
       <c r="C12" s="4">
         <v>11</v>
       </c>
-      <c r="D12" s="75">
+      <c r="D12" s="26">
         <v>11</v>
       </c>
-      <c r="E12" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="36"/>
-    </row>
-    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="28"/>
-      <c r="B13" s="28"/>
+      <c r="E12" s="43" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="45"/>
+    </row>
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="36"/>
+      <c r="B13" s="36"/>
       <c r="C13" s="5">
         <v>12</v>
       </c>
-      <c r="D13" s="76">
+      <c r="D13" s="27">
         <v>12</v>
       </c>
-      <c r="E13" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="33"/>
-    </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
-      <c r="B14" s="28"/>
+      <c r="E13" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="42"/>
+    </row>
+    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="36"/>
+      <c r="B14" s="36"/>
       <c r="C14" s="4">
         <v>13</v>
       </c>
-      <c r="D14" s="61">
+      <c r="D14" s="4">
         <v>13</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
-      <c r="B15" s="29"/>
+    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="37"/>
+      <c r="B15" s="37"/>
       <c r="C15" s="5">
         <v>14</v>
       </c>
-      <c r="D15" s="62">
+      <c r="D15" s="5">
         <v>14</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>17</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="B16" s="26" t="s">
-        <v>42</v>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" s="39" t="s">
+        <v>41</v>
       </c>
       <c r="C16" s="9">
         <v>15</v>
       </c>
-      <c r="D16" s="66">
+      <c r="D16" s="9">
         <v>15</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" s="39"/>
+      <c r="B17" s="39"/>
       <c r="C17" s="8">
         <v>16</v>
       </c>
-      <c r="D17" s="65">
+      <c r="D17" s="8">
         <v>16</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
     </row>
-    <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="B18" s="25" t="s">
-        <v>45</v>
+    <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="46" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="47" t="s">
+        <v>44</v>
       </c>
       <c r="C18" s="18">
         <v>17</v>
       </c>
-      <c r="D18" s="72">
+      <c r="D18" s="18">
         <v>1</v>
       </c>
       <c r="E18" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="F18" s="18" t="s">
-        <v>56</v>
-      </c>
       <c r="G18" s="18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H18" s="18"/>
       <c r="I18" s="18"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="24"/>
-      <c r="B19" s="25"/>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" s="46"/>
+      <c r="B19" s="47"/>
       <c r="C19" s="19">
         <v>18</v>
       </c>
-      <c r="D19" s="73">
+      <c r="D19" s="19">
         <v>2</v>
       </c>
       <c r="E19" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G19" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H19" s="19"/>
       <c r="I19" s="19"/>
     </row>
-    <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="77" t="s">
-        <v>59</v>
-      </c>
-      <c r="B20" s="78" t="s">
-        <v>38</v>
+    <row r="20" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="48" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="51" t="s">
+        <v>37</v>
       </c>
       <c r="C20" s="11">
         <v>19</v>
       </c>
-      <c r="D20" s="67">
+      <c r="D20" s="11">
         <v>3</v>
       </c>
       <c r="E20" s="11" t="s">
         <v>18</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G20" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H20" s="11"/>
       <c r="I20" s="11"/>
     </row>
-    <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="79"/>
-      <c r="B21" s="80"/>
+    <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="49"/>
+      <c r="B21" s="52"/>
       <c r="C21" s="12">
         <v>20</v>
       </c>
-      <c r="D21" s="68">
+      <c r="D21" s="12">
         <v>4</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>19</v>
       </c>
       <c r="F21" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G21" s="12" t="s">
         <v>36</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>37</v>
       </c>
       <c r="H21" s="12"/>
       <c r="I21" s="12"/>
     </row>
-    <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="81"/>
-      <c r="B22" s="82"/>
+    <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="50"/>
+      <c r="B22" s="53"/>
       <c r="C22" s="11">
         <v>21</v>
       </c>
-      <c r="D22" s="67">
+      <c r="D22" s="11">
         <v>5</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H22" s="11"/>
       <c r="I22" s="11"/>
     </row>
-    <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="83" t="s">
-        <v>61</v>
-      </c>
-      <c r="B23" s="84" t="s">
-        <v>44</v>
+    <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="33" t="s">
+        <v>43</v>
       </c>
       <c r="C23" s="15">
         <v>22</v>
       </c>
-      <c r="D23" s="70">
+      <c r="D23" s="15">
         <v>6</v>
       </c>
       <c r="E23" s="15" t="s">
         <v>1</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G23" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H23" s="15"/>
       <c r="I23" s="15"/>
     </row>
-    <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="85"/>
-      <c r="B24" s="86"/>
+    <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="32"/>
+      <c r="B24" s="34"/>
       <c r="C24" s="16">
         <v>23</v>
       </c>
-      <c r="D24" s="71">
+      <c r="D24" s="16">
         <v>7</v>
       </c>
       <c r="E24" s="16" t="s">
         <v>2</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G24" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H24" s="16"/>
       <c r="I24" s="16"/>
     </row>
-    <row r="25" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="17"/>
       <c r="B25" s="13"/>
       <c r="C25" s="14">
         <v>24</v>
       </c>
-      <c r="D25" s="69">
+      <c r="D25" s="14">
         <v>8</v>
       </c>
-      <c r="E25" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="39"/>
-      <c r="I25" s="39"/>
-    </row>
-    <row r="26" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E25" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" s="30"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="30"/>
+    </row>
+    <row r="26" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="17"/>
       <c r="B26" s="13"/>
       <c r="C26" s="14">
         <v>25</v>
       </c>
-      <c r="D26" s="69">
+      <c r="D26" s="14">
         <v>9</v>
       </c>
-      <c r="E26" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="39"/>
-    </row>
-    <row r="27" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E26" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" s="30"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="30"/>
+    </row>
+    <row r="27" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="17"/>
       <c r="B27" s="13"/>
       <c r="C27" s="14">
         <v>26</v>
       </c>
-      <c r="D27" s="69">
+      <c r="D27" s="14">
         <v>10</v>
       </c>
-      <c r="E27" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="F27" s="39"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="39"/>
-      <c r="I27" s="39"/>
-    </row>
-    <row r="28" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E27" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+    </row>
+    <row r="28" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="17"/>
       <c r="B28" s="13"/>
       <c r="C28" s="14">
         <v>27</v>
       </c>
-      <c r="D28" s="69">
+      <c r="D28" s="14">
         <v>11</v>
       </c>
-      <c r="E28" s="39" t="s">
-        <v>33</v>
-      </c>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="39"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="B29" s="38" t="s">
-        <v>39</v>
+      <c r="E28" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="F28" s="30"/>
+      <c r="G28" s="30"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="30"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="29" t="s">
+        <v>38</v>
       </c>
       <c r="C29" s="6">
         <v>28</v>
       </c>
-      <c r="D29" s="63">
+      <c r="D29" s="6">
         <v>12</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F29" s="6"/>
       <c r="G29" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="37"/>
-      <c r="B30" s="38"/>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30" s="28"/>
+      <c r="B30" s="29"/>
       <c r="C30" s="7">
         <v>29</v>
       </c>
-      <c r="D30" s="64">
+      <c r="D30" s="7">
         <v>13</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H30" s="7"/>
       <c r="I30" s="7"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="37"/>
-      <c r="B31" s="38"/>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31" s="28"/>
+      <c r="B31" s="29"/>
       <c r="C31" s="6">
         <v>30</v>
       </c>
-      <c r="D31" s="63">
+      <c r="D31" s="6">
         <v>14</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="37"/>
-      <c r="B32" s="38"/>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32" s="28"/>
+      <c r="B32" s="29"/>
       <c r="C32" s="7">
         <v>31</v>
       </c>
-      <c r="D32" s="64">
+      <c r="D32" s="7">
         <v>15</v>
       </c>
       <c r="E32" s="7" t="s">
@@ -2158,32 +2149,43 @@
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H32" s="7"/>
       <c r="I32" s="7"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="37"/>
-      <c r="B33" s="38"/>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A33" s="28"/>
+      <c r="B33" s="29"/>
       <c r="C33" s="6">
         <v>32</v>
       </c>
-      <c r="D33" s="63">
+      <c r="D33" s="6">
         <v>16</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F33" s="6"/>
       <c r="G33" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H33" s="6"/>
       <c r="I33" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A2:A15"/>
+    <mergeCell ref="B2:B15"/>
+    <mergeCell ref="E11:I11"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="E13:I13"/>
+    <mergeCell ref="E12:I12"/>
     <mergeCell ref="A29:A33"/>
     <mergeCell ref="B29:B33"/>
     <mergeCell ref="E26:I26"/>
@@ -2192,17 +2194,6 @@
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="E27:I27"/>
     <mergeCell ref="E28:I28"/>
-    <mergeCell ref="A2:A15"/>
-    <mergeCell ref="B2:B15"/>
-    <mergeCell ref="E11:I11"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="E13:I13"/>
-    <mergeCell ref="E12:I12"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="A16:A17"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2214,101 +2205,98 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{036672A4-8952-44C6-9E0D-0D4906E8D835}">
   <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="8" width="7.28515625" customWidth="1"/>
-    <col min="9" max="9" width="2.7109375" customWidth="1"/>
-    <col min="10" max="10" width="2.140625" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="8" width="7.26953125" customWidth="1"/>
+    <col min="9" max="9" width="2.7265625" customWidth="1"/>
+    <col min="10" max="10" width="2.1796875" customWidth="1"/>
+    <col min="11" max="11" width="10.54296875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.7109375" customWidth="1"/>
-    <col min="14" max="14" width="10.42578125" customWidth="1"/>
+    <col min="13" max="13" width="3.7265625" customWidth="1"/>
+    <col min="14" max="14" width="10.453125" customWidth="1"/>
     <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="7.28515625" customWidth="1"/>
-    <col min="18" max="18" width="7.28515625" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="7.28515625" customWidth="1"/>
+    <col min="16" max="17" width="7.26953125" customWidth="1"/>
+    <col min="18" max="18" width="7.26953125" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="7.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
-        <v>81</v>
-      </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="48" t="s">
-        <v>84</v>
-      </c>
-      <c r="L1" s="48"/>
-      <c r="N1" s="49" t="s">
-        <v>85</v>
-      </c>
-      <c r="O1" s="49"/>
-    </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="40" t="s">
+    <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="24"/>
+      <c r="K1" s="57" t="s">
+        <v>78</v>
+      </c>
+      <c r="L1" s="57"/>
+      <c r="N1" s="58" t="s">
+        <v>79</v>
+      </c>
+      <c r="O1" s="58"/>
+    </row>
+    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="58"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="24"/>
       <c r="K2" s="21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L2" s="21" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="N2" s="21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O2" s="21" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="Q2" s="20"/>
     </row>
-    <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="53">
+    <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="23">
         <v>1</v>
       </c>
-      <c r="B3" s="53">
+      <c r="B3" s="23">
         <v>2</v>
       </c>
-      <c r="C3" s="53">
+      <c r="C3" s="23">
         <v>3</v>
       </c>
-      <c r="D3" s="53">
+      <c r="D3" s="23">
         <v>4</v>
       </c>
-      <c r="E3" s="53">
+      <c r="E3" s="23">
         <v>5</v>
       </c>
-      <c r="F3" s="53">
+      <c r="F3" s="23">
         <v>6</v>
       </c>
-      <c r="G3" s="53">
+      <c r="G3" s="23">
         <v>7</v>
       </c>
-      <c r="H3" s="53">
+      <c r="H3" s="23">
         <v>8</v>
       </c>
-      <c r="I3" s="59"/>
-      <c r="J3" s="58"/>
+      <c r="I3" s="24"/>
       <c r="K3" s="21">
         <v>1</v>
       </c>
@@ -2323,33 +2311,32 @@
       </c>
       <c r="Q3" s="20"/>
     </row>
-    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="54" t="s">
+    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="54" t="s">
+      <c r="D4" s="55" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="54" t="s">
+      <c r="E4" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="54" t="s">
+      <c r="F4" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="54" t="s">
+      <c r="G4" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="54" t="s">
-        <v>66</v>
-      </c>
-      <c r="I4" s="59"/>
-      <c r="J4" s="58"/>
+      <c r="H4" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="I4" s="24"/>
       <c r="K4" s="21">
         <v>2</v>
       </c>
@@ -2364,143 +2351,130 @@
       </c>
       <c r="Q4" s="20"/>
     </row>
-    <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="54"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="58"/>
+    <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="55"/>
+      <c r="B5" s="55"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="55"/>
+      <c r="I5" s="24"/>
       <c r="K5" s="21">
         <v>3</v>
       </c>
       <c r="L5" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="N5" s="21">
         <v>3</v>
       </c>
       <c r="O5" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="Q5" s="20"/>
     </row>
-    <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="52"/>
-      <c r="B6" s="52"/>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52"/>
-      <c r="G6" s="52"/>
-      <c r="H6" s="52"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="58"/>
+    <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I6" s="24"/>
       <c r="K6" s="21">
         <v>4</v>
       </c>
       <c r="L6" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="N6" s="21">
         <v>4</v>
       </c>
       <c r="O6" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q6" s="20"/>
     </row>
-    <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="53">
+    <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="23">
         <v>9</v>
       </c>
-      <c r="B7" s="53">
+      <c r="B7" s="23">
         <v>10</v>
       </c>
-      <c r="C7" s="53">
+      <c r="C7" s="23">
         <v>11</v>
       </c>
-      <c r="D7" s="53">
+      <c r="D7" s="23">
         <v>12</v>
       </c>
-      <c r="E7" s="53">
+      <c r="E7" s="23">
         <v>13</v>
       </c>
-      <c r="F7" s="53">
+      <c r="F7" s="23">
         <v>14</v>
       </c>
-      <c r="G7" s="53">
+      <c r="G7" s="23">
         <v>15</v>
       </c>
-      <c r="H7" s="53">
+      <c r="H7" s="23">
         <v>16</v>
       </c>
-      <c r="I7" s="59"/>
-      <c r="J7" s="58"/>
+      <c r="I7" s="24"/>
       <c r="K7" s="21">
         <v>5</v>
       </c>
       <c r="L7" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N7" s="21">
         <v>5</v>
       </c>
       <c r="O7" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q7" s="20"/>
     </row>
-    <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="54" t="s">
-        <v>65</v>
-      </c>
-      <c r="B8" s="44"/>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="54" t="s">
-        <v>93</v>
-      </c>
-      <c r="F8" s="54" t="s">
+    <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="55" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="66"/>
+      <c r="C8" s="66"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="55" t="s">
+        <v>83</v>
+      </c>
+      <c r="F8" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="51" t="s">
-        <v>71</v>
-      </c>
-      <c r="H8" s="51" t="s">
+      <c r="G8" s="54" t="s">
         <v>70</v>
       </c>
-      <c r="I8" s="59"/>
-      <c r="J8" s="58"/>
+      <c r="H8" s="54" t="s">
+        <v>69</v>
+      </c>
+      <c r="I8" s="24"/>
       <c r="K8" s="21">
         <v>6</v>
       </c>
       <c r="L8" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="N8" s="21">
         <v>6</v>
       </c>
       <c r="O8" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q8" s="20"/>
     </row>
-    <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="54"/>
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="54"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="59"/>
-      <c r="J9" s="58"/>
+    <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="55"/>
+      <c r="B9" s="66"/>
+      <c r="C9" s="66"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="54"/>
+      <c r="I9" s="24"/>
       <c r="K9" s="21">
         <v>7</v>
       </c>
@@ -2515,17 +2489,8 @@
       </c>
       <c r="Q9" s="20"/>
     </row>
-    <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="52"/>
-      <c r="B10" s="52"/>
-      <c r="C10" s="52"/>
-      <c r="D10" s="52"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="52"/>
-      <c r="G10" s="52"/>
-      <c r="H10" s="52"/>
-      <c r="I10" s="59"/>
-      <c r="J10" s="58"/>
+    <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I10" s="24"/>
       <c r="K10" s="21">
         <v>8</v>
       </c>
@@ -2540,19 +2505,18 @@
       </c>
       <c r="Q10" s="20"/>
     </row>
-    <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="40" t="s">
+    <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="59"/>
-      <c r="J11" s="58"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="56"/>
+      <c r="H11" s="56"/>
+      <c r="I11" s="24"/>
       <c r="K11" s="21">
         <v>9</v>
       </c>
@@ -2567,33 +2531,32 @@
       </c>
       <c r="Q11" s="20"/>
     </row>
-    <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="53">
+    <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="23">
         <v>1</v>
       </c>
-      <c r="B12" s="53">
+      <c r="B12" s="23">
         <v>2</v>
       </c>
-      <c r="C12" s="53">
+      <c r="C12" s="23">
         <v>3</v>
       </c>
-      <c r="D12" s="53">
+      <c r="D12" s="23">
         <v>4</v>
       </c>
-      <c r="E12" s="53">
+      <c r="E12" s="23">
         <v>5</v>
       </c>
-      <c r="F12" s="53">
+      <c r="F12" s="23">
         <v>6</v>
       </c>
-      <c r="G12" s="53">
+      <c r="G12" s="23">
         <v>7</v>
       </c>
-      <c r="H12" s="53">
+      <c r="H12" s="23">
         <v>8</v>
       </c>
-      <c r="I12" s="59"/>
-      <c r="J12" s="58"/>
+      <c r="I12" s="24"/>
       <c r="K12" s="21">
         <v>10</v>
       </c>
@@ -2608,50 +2571,54 @@
       </c>
       <c r="Q12" s="20"/>
     </row>
-    <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="54" t="s">
-        <v>95</v>
-      </c>
-      <c r="B13" s="54" t="s">
-        <v>96</v>
-      </c>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="55" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" s="55" t="s">
-        <v>97</v>
-      </c>
-      <c r="I13" s="59"/>
-      <c r="J13" s="58"/>
+    <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="55" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="67" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="67" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="67" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="67" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="67" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="67" t="s">
+        <v>83</v>
+      </c>
+      <c r="H13" s="66"/>
+      <c r="I13" s="24"/>
       <c r="K13" s="21">
         <v>11</v>
       </c>
       <c r="L13" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N13" s="21">
         <v>11</v>
       </c>
       <c r="O13" s="21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q13" s="20"/>
     </row>
-    <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="54"/>
-      <c r="B14" s="54"/>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="55"/>
-      <c r="H14" s="55"/>
-      <c r="I14" s="59"/>
-      <c r="J14" s="58"/>
+    <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="55"/>
+      <c r="B14" s="68"/>
+      <c r="C14" s="68"/>
+      <c r="D14" s="68"/>
+      <c r="E14" s="68"/>
+      <c r="F14" s="68"/>
+      <c r="G14" s="68"/>
+      <c r="H14" s="66"/>
+      <c r="I14" s="24"/>
       <c r="K14" s="21">
         <v>12</v>
       </c>
@@ -2666,17 +2633,16 @@
       </c>
       <c r="Q14" s="20"/>
     </row>
-    <row r="15" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="57"/>
-      <c r="B15" s="57"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="57"/>
-      <c r="G15" s="57"/>
-      <c r="H15" s="57"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="58"/>
+    <row r="15" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="24"/>
       <c r="K15" s="21">
         <v>13</v>
       </c>
@@ -2691,17 +2657,8 @@
       </c>
       <c r="Q15" s="20"/>
     </row>
-    <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="56"/>
-      <c r="B16" s="56"/>
-      <c r="C16" s="56"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56"/>
-      <c r="G16" s="56"/>
-      <c r="H16" s="56"/>
-      <c r="I16" s="59"/>
-      <c r="J16" s="58"/>
+    <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I16" s="24"/>
       <c r="K16" s="21">
         <v>14</v>
       </c>
@@ -2716,61 +2673,59 @@
       </c>
       <c r="Q16" s="20"/>
     </row>
-    <row r="17" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="40" t="s">
-        <v>86</v>
-      </c>
-      <c r="B17" s="40"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="59"/>
-      <c r="J17" s="58"/>
+    <row r="17" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="56" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" s="56"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="56"/>
+      <c r="G17" s="56"/>
+      <c r="H17" s="56"/>
+      <c r="I17" s="24"/>
       <c r="K17" s="21">
         <v>15</v>
       </c>
       <c r="L17" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N17" s="21">
         <v>15</v>
       </c>
       <c r="O17" s="21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q17" s="20"/>
     </row>
-    <row r="18" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="40" t="s">
+    <row r="18" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="40"/>
-      <c r="C18" s="40"/>
-      <c r="D18" s="40"/>
-      <c r="E18" s="40"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="59"/>
-      <c r="J18" s="58"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="56"/>
+      <c r="G18" s="56"/>
+      <c r="H18" s="56"/>
+      <c r="I18" s="24"/>
       <c r="K18" s="21">
         <v>16</v>
       </c>
       <c r="L18" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N18" s="21">
         <v>16</v>
       </c>
       <c r="O18" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="Q18" s="20"/>
     </row>
-    <row r="19" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="23">
         <v>1</v>
       </c>
@@ -2795,8 +2750,7 @@
       <c r="H19" s="23">
         <v>8</v>
       </c>
-      <c r="I19" s="59"/>
-      <c r="J19" s="58"/>
+      <c r="I19" s="24"/>
       <c r="N19" s="21">
         <v>17</v>
       </c>
@@ -2804,31 +2758,30 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20" s="41" t="s">
-        <v>89</v>
-      </c>
-      <c r="C20" s="42" t="s">
+    <row r="20" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="62" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="42" t="s">
+      <c r="D20" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="42" t="s">
-        <v>68</v>
-      </c>
-      <c r="F20" s="45" t="s">
+      <c r="E20" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="F20" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="G20" s="45" t="s">
+      <c r="G20" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="H20" s="44"/>
-      <c r="I20" s="59"/>
-      <c r="J20" s="58"/>
+      <c r="H20" s="66"/>
+      <c r="I20" s="24"/>
       <c r="N20" s="21">
         <v>18</v>
       </c>
@@ -2836,17 +2789,16 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="41"/>
-      <c r="B21" s="41"/>
-      <c r="C21" s="42"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="45"/>
-      <c r="G21" s="45"/>
-      <c r="H21" s="44"/>
-      <c r="I21" s="59"/>
-      <c r="J21" s="58"/>
+    <row r="21" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="62"/>
+      <c r="B21" s="62"/>
+      <c r="C21" s="63"/>
+      <c r="D21" s="63"/>
+      <c r="E21" s="63"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="64"/>
+      <c r="H21" s="66"/>
+      <c r="I21" s="24"/>
       <c r="N21" s="21">
         <v>19</v>
       </c>
@@ -2854,9 +2806,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I22" s="59"/>
-      <c r="J22" s="58"/>
+    <row r="22" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I22" s="24"/>
       <c r="N22" s="21">
         <v>20</v>
       </c>
@@ -2864,7 +2815,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="23">
         <v>9</v>
       </c>
@@ -2889,8 +2840,7 @@
       <c r="H23" s="23">
         <v>16</v>
       </c>
-      <c r="I23" s="59"/>
-      <c r="J23" s="58"/>
+      <c r="I23" s="24"/>
       <c r="N23" s="21">
         <v>21</v>
       </c>
@@ -2898,27 +2848,26 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="44"/>
-      <c r="B24" s="44"/>
-      <c r="C24" s="44"/>
-      <c r="D24" s="43" t="s">
+    <row r="24" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="66"/>
+      <c r="B24" s="66"/>
+      <c r="C24" s="66"/>
+      <c r="D24" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="E24" s="43" t="s">
+      <c r="E24" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="F24" s="43" t="s">
+      <c r="F24" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="G24" s="43" t="s">
+      <c r="G24" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="H24" s="43" t="s">
+      <c r="H24" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="I24" s="59"/>
-      <c r="J24" s="58"/>
+      <c r="I24" s="24"/>
       <c r="N24" s="21">
         <v>22</v>
       </c>
@@ -2926,25 +2875,25 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="44"/>
-      <c r="B25" s="44"/>
-      <c r="C25" s="44"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="43"/>
-      <c r="H25" s="43"/>
-      <c r="I25" s="59"/>
-      <c r="J25" s="58"/>
+    <row r="25" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="66"/>
+      <c r="B25" s="66"/>
+      <c r="C25" s="66"/>
+      <c r="D25" s="65"/>
+      <c r="E25" s="65"/>
+      <c r="F25" s="65"/>
+      <c r="G25" s="65"/>
+      <c r="H25" s="65"/>
+      <c r="I25" s="24"/>
       <c r="N25" s="21">
         <v>23</v>
       </c>
-      <c r="O25" s="21"/>
-    </row>
-    <row r="26" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I26" s="59"/>
-      <c r="J26" s="58"/>
+      <c r="O25" s="21" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I26" s="24"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
@@ -2954,26 +2903,26 @@
       <c r="O26" s="21"/>
       <c r="P26" s="2"/>
     </row>
-    <row r="27" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="40" t="s">
+    <row r="27" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="40"/>
-      <c r="C27" s="40"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="40"/>
-      <c r="F27" s="40"/>
-      <c r="G27" s="40"/>
-      <c r="H27" s="40"/>
-      <c r="I27" s="59"/>
-      <c r="J27" s="60"/>
+      <c r="B27" s="56"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="56"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="56"/>
+      <c r="G27" s="56"/>
+      <c r="H27" s="56"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="25"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
     </row>
-    <row r="28" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="23">
         <v>1</v>
       </c>
@@ -2998,124 +2947,164 @@
       <c r="H28" s="23">
         <v>8</v>
       </c>
-      <c r="I28" s="59"/>
-      <c r="J28" s="58"/>
-      <c r="K28" s="50" t="s">
+      <c r="I28" s="24"/>
+      <c r="K28" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="L28" s="50"/>
-      <c r="M28" s="50"/>
-      <c r="N28" s="50"/>
-      <c r="O28" s="50"/>
-    </row>
-    <row r="29" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="45" t="s">
-        <v>76</v>
-      </c>
-      <c r="B29" s="45" t="s">
-        <v>77</v>
-      </c>
-      <c r="C29" s="43" t="s">
-        <v>74</v>
-      </c>
-      <c r="D29" s="43" t="s">
-        <v>75</v>
-      </c>
-      <c r="E29" s="41" t="s">
+      <c r="L28" s="59"/>
+      <c r="M28" s="59"/>
+      <c r="N28" s="59"/>
+      <c r="O28" s="59"/>
+    </row>
+    <row r="29" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="69" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="F29" s="41" t="s">
-        <v>91</v>
-      </c>
-      <c r="G29" s="42" t="s">
-        <v>87</v>
-      </c>
-      <c r="H29" s="42" t="s">
-        <v>88</v>
-      </c>
-      <c r="I29" s="59"/>
-      <c r="J29" s="58"/>
+      <c r="C29" s="71" t="s">
+        <v>92</v>
+      </c>
+      <c r="D29" s="72" t="s">
+        <v>93</v>
+      </c>
+      <c r="E29" s="73" t="s">
+        <v>94</v>
+      </c>
+      <c r="F29" s="74"/>
+      <c r="G29" s="75" t="s">
+        <v>9</v>
+      </c>
+      <c r="H29" s="75" t="s">
+        <v>85</v>
+      </c>
+      <c r="I29" s="24"/>
       <c r="K29" s="10">
         <v>1</v>
       </c>
-      <c r="L29" s="46" t="s">
-        <v>21</v>
-      </c>
-      <c r="M29" s="46"/>
-      <c r="N29" s="46"/>
-      <c r="O29" s="46"/>
-    </row>
-    <row r="30" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="45"/>
-      <c r="B30" s="45"/>
-      <c r="C30" s="43"/>
-      <c r="D30" s="43"/>
-      <c r="E30" s="41"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="42"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="59"/>
-      <c r="J30" s="58"/>
+      <c r="L29" s="60" t="s">
+        <v>87</v>
+      </c>
+      <c r="M29" s="60"/>
+      <c r="N29" s="60"/>
+      <c r="O29" s="60"/>
+    </row>
+    <row r="30" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="69"/>
+      <c r="B30" s="70"/>
+      <c r="C30" s="71"/>
+      <c r="D30" s="72"/>
+      <c r="E30" s="73"/>
+      <c r="F30" s="74"/>
+      <c r="G30" s="75"/>
+      <c r="H30" s="75"/>
+      <c r="I30" s="24"/>
       <c r="K30" s="3">
         <v>2</v>
       </c>
-      <c r="L30" s="47" t="s">
-        <v>79</v>
-      </c>
-      <c r="M30" s="47"/>
-      <c r="N30" s="47"/>
-      <c r="O30" s="47"/>
-    </row>
-    <row r="31" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I31" s="59"/>
-      <c r="J31" s="58"/>
+      <c r="L30" s="61" t="s">
+        <v>88</v>
+      </c>
+      <c r="M30" s="61"/>
+      <c r="N30" s="61"/>
+      <c r="O30" s="61"/>
+    </row>
+    <row r="31" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I31" s="24"/>
       <c r="K31" s="10">
         <v>3</v>
       </c>
-      <c r="L31" s="46" t="s">
-        <v>80</v>
-      </c>
-      <c r="M31" s="46"/>
-      <c r="N31" s="46"/>
-      <c r="O31" s="46"/>
-    </row>
-    <row r="32" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I32" s="59"/>
-      <c r="J32" s="58"/>
+      <c r="L31" s="60" t="s">
+        <v>74</v>
+      </c>
+      <c r="M31" s="60"/>
+      <c r="N31" s="60"/>
+      <c r="O31" s="60"/>
+    </row>
+    <row r="32" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I32" s="24"/>
       <c r="K32" s="3">
         <v>4</v>
       </c>
-      <c r="L32" s="47" t="s">
-        <v>92</v>
-      </c>
-      <c r="M32" s="47"/>
-      <c r="N32" s="47"/>
-      <c r="O32" s="47"/>
-    </row>
-    <row r="33" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I33" s="59"/>
-      <c r="J33" s="58"/>
+      <c r="L32" s="61" t="s">
+        <v>82</v>
+      </c>
+      <c r="M32" s="61"/>
+      <c r="N32" s="61"/>
+      <c r="O32" s="61"/>
+    </row>
+    <row r="33" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I33" s="24"/>
       <c r="K33" s="10">
         <v>5</v>
       </c>
-      <c r="L33" s="46"/>
-      <c r="M33" s="46"/>
-      <c r="N33" s="46"/>
-      <c r="O33" s="46"/>
-    </row>
-    <row r="34" spans="9:15" x14ac:dyDescent="0.25">
-      <c r="I34" s="59"/>
-      <c r="J34" s="58"/>
+      <c r="L33" s="60" t="s">
+        <v>89</v>
+      </c>
+      <c r="M33" s="60"/>
+      <c r="N33" s="60"/>
+      <c r="O33" s="60"/>
+    </row>
+    <row r="34" spans="9:15" x14ac:dyDescent="0.35">
+      <c r="I34" s="24"/>
       <c r="K34" s="3">
         <v>6</v>
       </c>
-      <c r="L34" s="47"/>
-      <c r="M34" s="47"/>
-      <c r="N34" s="47"/>
-      <c r="O34" s="47"/>
+      <c r="L34" s="61"/>
+      <c r="M34" s="61"/>
+      <c r="N34" s="61"/>
+      <c r="O34" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="63">
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="A18:H18"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="L31:O31"/>
+    <mergeCell ref="L32:O32"/>
+    <mergeCell ref="L33:O33"/>
+    <mergeCell ref="L34:O34"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="K28:O28"/>
+    <mergeCell ref="L29:O29"/>
+    <mergeCell ref="L30:O30"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="A11:H11"/>
@@ -3129,56 +3118,9 @@
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="H4:H5"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="K28:O28"/>
-    <mergeCell ref="L29:O29"/>
-    <mergeCell ref="L30:O30"/>
-    <mergeCell ref="L31:O31"/>
-    <mergeCell ref="L32:O32"/>
-    <mergeCell ref="L33:O33"/>
-    <mergeCell ref="L34:O34"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="A27:H27"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
     <mergeCell ref="H8:H9"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="A18:H18"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:E9"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>